<commit_message>
aggiunto meccanismo di blocco al rversamento della terminologia flaggata come 'hide' nello switch dell'admin.
</commit_message>
<xml_diff>
--- a/static/saved_dataframes/Terminologia_metaglossario.xlsx
+++ b/static/saved_dataframes/Terminologia_metaglossario.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z71"/>
+  <dimension ref="A1:Z68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2511,27 +2511,39 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Mezzi Straordinari</t>
+          <t>Suscettività Da Frana</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Termine che indica il denaro del fondo emergenza nazionale.</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+          <t>Può intendersi la stima – quantitativa o qualitativa – della tipologia, del volume (o dell’area) nonché della distribuzione delle frane esistenti o che potrebbero verificarsi all’interno di una ben determinata area. La suscettibilità potrebbe anche includere una descrizione della velocità e della intensità delle frane esistenti o potenziali.</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Geologia e sismologia</t>
+        </is>
+      </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Tommaso Sansone</t>
+          <t>Robin Fell , Jordi Corominas , Christophe Bonnard , Leonardo Cascini , Eric Leroi , William Z. Savage, Per Conto Del Jtc-1 Joint Technical Committee On Landslides And Engineered Slopes</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Linee Guida Per La Zonazione Della Suscettibilità, Della Pericolosità E Del Rischio Da Frana Ai Fini Della Pianificazione Territoriale</t>
+        </is>
+      </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>http://www.associazionegeotecnica.it/sites/default/files/linee_guida_jtc-1_italiano_agi.pdf</t>
+        </is>
+      </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr"/>
@@ -2545,11 +2557,11 @@
       <c r="W32" t="inlineStr"/>
       <c r="X32" t="inlineStr"/>
       <c r="Y32" s="2" t="n">
-        <v>43412</v>
+        <v>43119</v>
       </c>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>IDF1008657</t>
+          <t>IDF1008675</t>
         </is>
       </c>
     </row>
@@ -2557,59 +2569,63 @@
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Suscettività Da Frana</t>
-        </is>
-      </c>
+      <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Può intendersi la stima – quantitativa o qualitativa – della tipologia, del volume (o dell’area) nonché della distribuzione delle frane esistenti o che potrebbero verificarsi all’interno di una ben determinata area. La suscettibilità potrebbe anche includere una descrizione della velocità e della intensità delle frane esistenti o potenziali.</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Geologia e sismologia</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Robin Fell , Jordi Corominas , Christophe Bonnard , Leonardo Cascini , Eric Leroi , William Z. Savage, Per Conto Del Jtc-1 Joint Technical Committee On Landslides And Engineered Slopes</t>
-        </is>
-      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>Linee Guida Per La Zonazione Della Suscettibilità, Della Pericolosità E Del Rischio Da Frana Ai Fini Della Pianificazione Territoriale</t>
-        </is>
-      </c>
+      <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>http://www.associazionegeotecnica.it/sites/default/files/linee_guida_jtc-1_italiano_agi.pdf</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>Centrale nazionale d'allarme</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>CENAL</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>La CENAL, una divisione dell'Ufficio federale della protezione della popolazione (UFPP), è l'organo federale competente per gli eventi straordinari. Il compito principale della CENAL è quello di tracciare il quadro della situazione prioritaria per la protezione della popolazione. A tal fine, sia nella quotidianità che in caso d'evento scambia informazioni con le autorità competenti dei Cantoni, diversi uffici federali, i gestori delle reti di telecomunicazione, dell'energia e dei trasporti, organizzazioni internazionali e con i centri d'analisi della situazione dei Paesi limitrofi. In caso d'evento, funge da primo punto di contatto per i Cantoni in relazione a tutte le questioni inerenti alla protezione della popolazione. In caso di eventi maggiori, la CENAL informa lo stato maggiore federale Protezione della popolazione e l'assiste nel suo lavoro.</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>Competenza di protezione civile</t>
+        </is>
+      </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr"/>
-      <c r="T33" t="inlineStr"/>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>Benvenuti sul sito web della Centrale nazionale d'allarme CENAL</t>
+        </is>
+      </c>
       <c r="U33" t="inlineStr"/>
-      <c r="V33" t="inlineStr"/>
-      <c r="W33" t="inlineStr"/>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t>Confederazione Elvetica</t>
+        </is>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>https://www.naz.ch/index_it.html</t>
+        </is>
+      </c>
       <c r="X33" t="inlineStr"/>
       <c r="Y33" s="2" t="n">
-        <v>43119</v>
+        <v>43656</v>
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>IDF1008675</t>
+          <t>ITCH00001</t>
         </is>
       </c>
     </row>
@@ -2617,11 +2633,7 @@
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>lemma it1</t>
-        </is>
-      </c>
+      <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
@@ -2634,30 +2646,56 @@
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr">
         <is>
-          <t>lemma ch1</t>
-        </is>
-      </c>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
+          <t>Stato maggiore federale Protezione della popolazione</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>SMFP</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>Nel caso in cui si delinea o si è verificato un evento di portata nazionale rilevante per la protezione della popolazione, lo SMFP assume i compiti seguenti (art. 4, cpv. 2 OSMFP):
+- assicura lo scambio di informazioni e il coordinamento con altri stati maggiori e organi della Confederazione e dei Cantoni, con i gestori di infrastrutture critiche e con i competenti organi all'estero;
+riunisce le situazioni settoriali e parziali per ottenere un quadro generale della situazione e ne effettua la valutazione.
+- elabora le basi decisionali all’attenzione del Consiglio federale, del dipartimento o dell’ufficio competente;
+- coordina le conoscenze degli esperti a livello federale;
+- coordina l'impiego delle risorse nazionali e internazionali.
+Lo SMFP si compone di una conferenza dei direttori, un elemento di pianificazione formato da esperti degli organi competenti e un elemento d'intervento e di supporto.</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>Competenza di protezione civile</t>
+        </is>
+      </c>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr"/>
-      <c r="T34" t="inlineStr"/>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>Elemento d'intervento e di supporto dello Stato maggiore federale Protezione della popolazione</t>
+        </is>
+      </c>
       <c r="U34" t="inlineStr"/>
-      <c r="V34" t="inlineStr"/>
-      <c r="W34" t="inlineStr"/>
-      <c r="X34" t="inlineStr">
-        <is>
-          <t>prova</t>
-        </is>
-      </c>
+      <c r="V34" t="inlineStr">
+        <is>
+          <t>Confederazione Elvetica</t>
+        </is>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>https://www.naz.ch/it/naz/eo.html</t>
+        </is>
+      </c>
+      <c r="X34" t="inlineStr"/>
       <c r="Y34" s="2" t="n">
-        <v>43866</v>
+        <v>43656</v>
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>ITCH00000</t>
+          <t>ITCH00002</t>
         </is>
       </c>
     </row>
@@ -2665,64 +2703,107 @@
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" t="inlineStr"/>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Protezione civile</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Competenza di protezione civile</t>
+        </is>
+      </c>
       <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Art 1, comma 1</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=1&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=1&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Presidenza Del Consiglio Dei Ministri</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Gazzetta Ufficiale</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>http://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
+        </is>
+      </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>sezione del militare e della protezione della popolazione</t>
-        </is>
-      </c>
-      <c r="N35" t="inlineStr">
-        <is>
-          <t>SMPP</t>
-        </is>
-      </c>
+          <t>Protezione civile</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr">
         <is>
-          <t>La Sezione è articolata in cinque servizi con distinte aree di competenza: il Servizio amministrativo, il Servizio degli affari militari e del comando di circondario, il Servizio della protezione civile, il Servizio costruzioni di protezione civile e il Servizio della protezione della popolazione. 
-Il servizio amministrativo centralizzato della sezione si occupa di fornire le prime informazioni all’utenza e di smistarle ai vari servizi di competenza. Altri compiti specifici sono la contabilità, la corrispondenza e il supporto logistico per tutta la sezione. 
-Il Servizio degli affari militari e comando di circondario si occupa delle pratiche amministrative legate ai servizi d’istruzione dei militi domiciliati in Ticino come pure degli obblighi fuori servizio (tiro obbligatorio, obbligo di notifica), tiene il controllo dei dati di servizio e di quelli personali dei militi con la collaborazione degli uffici di controllo abitanti dei comuni. 
-Il Servizio della protezione civile, unitamente al Centro istruzione della protezione civile di Rivera, assicura l'applicazione delle norme federali e cantonali di protezione civile nelle regioni e nei comuni, cura le diverse pianificazioni (allarmi, approvvigionamenti,...) e l'istruzione dei militi astretti.
-Il Servizio costruzioni si occupa della pianificazione e gestione dei posti protetti, come pure della realizzazione delle costruzioni protette (rifugi, impianti regionali).
-Il servizio della protezione della popolazione si occupa prevalentemente dei preparativi per i casi di emergenza e di catastrofe.</t>
-        </is>
-      </c>
-      <c r="P35" t="inlineStr"/>
+          <t>La protezione civile protegge la popolazione, assiste le persone in cerca di protezione, protegge i beni culturali, sostiene gli organi di condotta e le altre organizzazioni partner nonché svolge lavori di ripristino e di pubblica utilità. Essa è un’organizzazione civile che opera singolarmente o in maniera coordinata, come organizzazione partner, all'interno della struttura svizzera di di protezione della popolazione.</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>Competenza di protezione civile</t>
+        </is>
+      </c>
       <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="inlineStr"/>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>Art. 1</t>
+        </is>
+      </c>
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr">
         <is>
-          <t>Chi siamo</t>
+          <t>Legge sulla protezione civile del 26 febbraio 2007</t>
         </is>
       </c>
       <c r="U35" t="inlineStr"/>
       <c r="V35" t="inlineStr">
         <is>
-          <t>Repubblica e Canton Ticino</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
       <c r="W35" t="inlineStr">
         <is>
-          <t>https://www4.ti.ch/di/smpp/chi-siamo/presentazione/</t>
-        </is>
-      </c>
-      <c r="X35" t="inlineStr"/>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/44</t>
+        </is>
+      </c>
+      <c r="X35" t="inlineStr">
+        <is>
+          <t>Definizioni riorganizzate da Tommaso Sansone, Politecnico di Milano.</t>
+        </is>
+      </c>
       <c r="Y35" s="2" t="n">
-        <v>43845</v>
+        <v>43656</v>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>ITCH00000</t>
+          <t>ITCH00003</t>
         </is>
       </c>
     </row>
@@ -2730,55 +2811,64 @@
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>SOREU dei laghi</t>
-        </is>
-      </c>
+      <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>La SOREU dei Laghi è il riferimento per i territori di Como, Varese, Lecco e l'area del Legnanese.</t>
-        </is>
-      </c>
+      <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>SOREU dei Laghi</t>
-        </is>
-      </c>
+      <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>Areu Lombardia</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>https://www.areu.lombardia.it/web/home/soreu-dei-laghi</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Comando della protezione civile</t>
+        </is>
+      </c>
       <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Il comando della protezione civile è l’organo che dirige la protezione civile, ed è generalmente costituito dal comandante della protezione civile e dai suoi sostituti. I suoi compiti fondamentali sono i seguenti:
+- condurre gli interventi
+- condurre la protezione civile dal punto di vista organizzativo, amministrativo, del personale e del materiale
+- preparare, svolgere e valutare i corsi di ripetizione
+- assicurare l’efficienza operativa di costruzioni di protezione, materiale e infrastrutture per la diffusione dell’allarme
+- rappresentare le questioni della protezione civile presso le autorità, le organizzazioni partner, gli organi di condotta e la popolazione</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>Competenza di protezione civile</t>
+        </is>
+      </c>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr"/>
-      <c r="T36" t="inlineStr"/>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>Il comando della protezione civile</t>
+        </is>
+      </c>
       <c r="U36" t="inlineStr"/>
-      <c r="V36" t="inlineStr"/>
-      <c r="W36" t="inlineStr"/>
+      <c r="V36" t="inlineStr">
+        <is>
+          <t>Confederazione Elvetica</t>
+        </is>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>https://www.babs.admin.ch/it/zs/org/kdo.html</t>
+        </is>
+      </c>
       <c r="X36" t="inlineStr"/>
       <c r="Y36" s="2" t="n">
-        <v>43844</v>
+        <v>43656</v>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>ITCH00000</t>
+          <t>ITCH00004</t>
         </is>
       </c>
     </row>
@@ -2786,59 +2876,63 @@
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Sala Operativa Regionale dell'Emergenza Urgenza</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>SOREU</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Le SOREU hanno valenza interprovinciale: gestiscono le chiamate di soccorso sanitario con l'invio dei mezzi più appropriati fino al completamento del soccorso e/o all'eventuale affidamento del paziente alle strutture ospedaliere più idonee. Le SOREU operano tramite le dotazioni tecnologiche assegnate da AREU che permettono loro una costante interconnessione con i Call Center NUE 112 di riferimento, con i mezzi di soccorso delle AAT della propria area di competenza e con i Call Center sanitari specialistici, in modo da ottimizzare i tempi di risposta e intervento.</t>
-        </is>
-      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>Le SOREU</t>
-        </is>
-      </c>
+      <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>Areu Lombardia</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>https://www.areu.lombardia.it/web/home/soreu</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>Impianto di protezione per la protezione della popolazione</t>
+        </is>
+      </c>
       <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr"/>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Si definiscono impianti di protezione i posti di comando, gli impianti d'apprestamento, i centri sanitari protetti e gli ospedali protetti. Essi vengono utilizzati soprattutto per garantire la condotta e l’operatività dei mezzi della protezione della popolazione.</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>Competenza di protezione civile</t>
+        </is>
+      </c>
       <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr"/>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>Impianti di protezione per la protezione della popolazione</t>
+        </is>
+      </c>
       <c r="S37" t="inlineStr"/>
-      <c r="T37" t="inlineStr"/>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>Costruzioni di protezione</t>
+        </is>
+      </c>
       <c r="U37" t="inlineStr"/>
-      <c r="V37" t="inlineStr"/>
-      <c r="W37" t="inlineStr"/>
+      <c r="V37" t="inlineStr">
+        <is>
+          <t>Confederazione Elvetica</t>
+        </is>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>https://www.babs.admin.ch/it/aufgabenbabs/schutzbauten.html</t>
+        </is>
+      </c>
       <c r="X37" t="inlineStr"/>
       <c r="Y37" s="2" t="n">
-        <v>43844</v>
+        <v>43657</v>
       </c>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>ITCH00000</t>
+          <t>ITCH00005</t>
         </is>
       </c>
     </row>
@@ -2846,21 +2940,9 @@
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Nucleo Unitario di Valutazione e Risposta Emergenze transfrontaliere</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>NUVRE</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>team transfrontaliero di coordinamento costituito congiuntamente da personale qualificato, formato e attrezzato, della protezione civile lombarda e ticinese. Esso ha il compito, durante le emergenze nei territori di confine, di operare insieme sia per la valutazione dell’evento in corso e per i reciproci possibili riflessi sui rispettivi territori, sia quali “ufficiali di collegamento” per collegare le rispettive sale operative di ambo i lati del confine, consentendo una efficiente ed efficace relazione operativa. Il NUVRE viene introdotto dal progetto Gestisco 2018-2021.</t>
-        </is>
-      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
@@ -2869,24 +2951,59 @@
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr"/>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Evento NBC</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>NBC</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>Per evento NBC s'intende l'emissione illecita di sostanze nucleari (atomiche e radiologiche, N), biologiche (B) o chimiche (C). L'emissione può essere accidentale (incidente) o intenzionale (atto criminale o terroristico). Si distinguono i seguenti settori:
+- settore N: emissione di radiazioni ionizzanti e radioattività;
+- settore B: emissione di organismi patogeni (che causano malattie) o dei loro prodotti metabolici;
+- settore C: emissione di gas, liquidi o solidi tossici.</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>Competenza di protezione civile</t>
+        </is>
+      </c>
       <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr"/>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>Definizione di „evento NBC“: emissione di sostanze pericolose</t>
+        </is>
+      </c>
       <c r="S38" t="inlineStr"/>
-      <c r="T38" t="inlineStr"/>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>La Protezione NBC</t>
+        </is>
+      </c>
       <c r="U38" t="inlineStr"/>
-      <c r="V38" t="inlineStr"/>
-      <c r="W38" t="inlineStr"/>
+      <c r="V38" t="inlineStr">
+        <is>
+          <t>Confederazione Elvetica</t>
+        </is>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>https://www.babs.admin.ch/it/aufgabenbabs/abcschutz.html</t>
+        </is>
+      </c>
       <c r="X38" t="inlineStr"/>
       <c r="Y38" s="2" t="n">
-        <v>43774</v>
+        <v>43657</v>
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>ITCH00000</t>
+          <t>ITCH00006</t>
         </is>
       </c>
     </row>
@@ -2896,24 +3013,48 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>lemma 23</t>
+          <t>Suscettibilità da Frana</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>La suscettibilità da frana è la probabilità che una frana avvenga in un territorio, sulla base delle condizioni locali. E’ una misura del grado in cui un territorio potrà essere interessato da frane, ossia una stima di “dove” le frane potranno accadere. La suscettibilità non considera la ricorrenza temporale, né la dimensione delle frane. In termini matematici, la suscettibilità da frana è comunemente espressa come la probabilità d’occorrenza spaziale di un dissesto, dato un insieme di condizioni territoriali e ambientali.</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Geologia e sismologia</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>primo paragrafo</t>
+        </is>
+      </c>
       <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr"/>
-      <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>lemma 24</t>
-        </is>
-      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Modelli e carte di suscettibilità da frana</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>IRPI</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>IRPI CNR</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>http://www.irpi.cnr.it/focus/suscettibilita-da-frana/</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr"/>
@@ -2924,17 +3065,13 @@
       <c r="U39" t="inlineStr"/>
       <c r="V39" t="inlineStr"/>
       <c r="W39" t="inlineStr"/>
-      <c r="X39" t="inlineStr">
-        <is>
-          <t>prova n1</t>
-        </is>
-      </c>
+      <c r="X39" t="inlineStr"/>
       <c r="Y39" s="2" t="n">
-        <v>43866</v>
+        <v>43731</v>
       </c>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>ITCH00000</t>
+          <t>ITCH00007</t>
         </is>
       </c>
     </row>
@@ -2949,48 +3086,100 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>VVF</t>
+          <t>VVFF</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Struttura operativa della protezione civile.</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr"/>
+          <t>In occasione degli eventi calamitosi, il Corpo nazionale dei vigili del fuoco opera gli interventi di soccorso tecnico indifferibili e urgenti: di ricerca e salvataggio delle persone e – ai fini della salvaguardia della pubblica incolumità – anche di messa in sicurezza dei luoghi, delle strutture e degli impianti.</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Competenza di soccorso tecnico urgente; Competenza della Protezione Civile</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Art. 10</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=10&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=3&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0#art</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
+        </is>
+      </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Alberto Bruno, Funzionario della protezione civile di regione lombardia</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr"/>
-      <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr"/>
+          <t>Presidenza Del Consiglio Dei Ministri</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Gazzetta Ufficiale</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>https://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>Pompieri</t>
+        </is>
+      </c>
       <c r="N40" t="inlineStr"/>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Componente della protezione civile, costituiscono corpo civico</t>
-        </is>
-      </c>
-      <c r="P40" t="inlineStr"/>
+          <t>I pompieri sono responsabili di salvataggio e lotta contro i sinistri in generale, compresa la lotta antincendio e contro i sinistri ordinari. Intervengono anche in caso d’emissioni tossiche, fuoriuscite di carburanti e contaminazioni radioattive. Sono un mezzo di primo intervento.</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>Competenza di soccorso tecnico urgente; Competenza della Protezione Civile</t>
+        </is>
+      </c>
       <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr"/>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>Art. 3</t>
+        </is>
+      </c>
       <c r="S40" t="inlineStr"/>
-      <c r="T40" t="inlineStr"/>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
+        </is>
+      </c>
       <c r="U40" t="inlineStr"/>
-      <c r="V40" t="inlineStr"/>
-      <c r="W40" t="inlineStr"/>
-      <c r="X40" t="inlineStr"/>
+      <c r="V40" t="inlineStr">
+        <is>
+          <t>Confederazione Elvetica</t>
+        </is>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+        </is>
+      </c>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>Per il lato italiano, definizione tratta dall'art 10 del codice di protezione civile del 2-1-2018, rielaborata da Tommaso Sansone.</t>
+        </is>
+      </c>
       <c r="Y40" s="2" t="n">
-        <v>43804</v>
+        <v>43766</v>
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>ITCH00000</t>
+          <t>ITCH00009</t>
         </is>
       </c>
     </row>
@@ -2998,63 +3187,107 @@
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="inlineStr"/>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Struttura operativa</t>
+        </is>
+      </c>
       <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Oltre al Corpo nazionale dei vigili del fuoco, che opera quale componente fondamentale del Servizio nazionale della protezione civile, sono strutture operative nazionali: a) le Forze armate; b) le Forze di polizia; c) gli enti e istituti di ricerca di rilievo nazionale con finalità di protezione civile, anche organizzati come centri di competenza, l'Istituto nazionale di geofisica e vulcanologia e il Consiglio nazionale delle ricerche; d) le strutture del Servizio sanitario nazionale; e) il volontariato organizzato di protezione civile iscritto nell'elenco nazionale del volontariato di protezione civile, l'Associazione della Croce rossa italiana e il Corpo nazionale del soccorso alpino e speleologico; f) il Sistema nazionale per la protezione dell'ambiente; g) le strutture preposte alla gestione dei servizi meteorologici a livello nazionale.</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Competenza della Protezione Civile</t>
+        </is>
+      </c>
       <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Art. 13</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=13&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=3&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0#art</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Presidenza Del Consiglio Dei Ministri</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Gazzetta Ufficiale</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>https://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
+        </is>
+      </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>Centrale nazionale d'allarme</t>
-        </is>
-      </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>CENAL</t>
-        </is>
-      </c>
+          <t>Organizzazione partner</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr">
         <is>
-          <t>La CENAL, una divisione dell'Ufficio federale della protezione della popolazione (UFPP), è l'organo federale competente per gli eventi straordinari. Il compito principale della CENAL è quello di tracciare il quadro della situazione prioritaria per la protezione della popolazione. A tal fine, sia nella quotidianità che in caso d'evento scambia informazioni con le autorità competenti dei Cantoni, diversi uffici federali, i gestori delle reti di telecomunicazione, dell'energia e dei trasporti, organizzazioni internazionali e con i centri d'analisi della situazione dei Paesi limitrofi. In caso d'evento, funge da primo punto di contatto per i Cantoni in relazione a tutte le questioni inerenti alla protezione della popolazione. In caso di eventi maggiori, la CENAL informa lo stato maggiore federale Protezione della popolazione e l'assiste nel suo lavoro.</t>
-        </is>
-      </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>Competenza di protezione civile</t>
-        </is>
-      </c>
-      <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr"/>
+          <t>Sono organizzazioni partner quelle che collaborano alla protezione della popolazione: Polizia, pompieri, servizi della sanità pubblica, servizi tecnici, protezione civile.</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>confederazione elvetica</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>Art. 3</t>
+        </is>
+      </c>
       <c r="S41" t="inlineStr"/>
       <c r="T41" t="inlineStr">
         <is>
-          <t>Benvenuti sul sito web della Centrale nazionale d'allarme CENAL</t>
-        </is>
-      </c>
-      <c r="U41" t="inlineStr"/>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
+        </is>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>Confederazion elvetica</t>
+        </is>
+      </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>Confederazione Elvetica</t>
+          <t>Confederazione elvetica</t>
         </is>
       </c>
       <c r="W41" t="inlineStr">
         <is>
-          <t>https://www.naz.ch/index_it.html</t>
-        </is>
-      </c>
-      <c r="X41" t="inlineStr"/>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+        </is>
+      </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>strutture operative in italia e organizzazioni partner in svizzera hanno la stessa connotazione all'interno di un sistema di protezione della popolazione.</t>
+        </is>
+      </c>
       <c r="Y41" s="2" t="n">
-        <v>43656</v>
+        <v>43766</v>
       </c>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>ITCH00001</t>
+          <t>ITCH00010</t>
         </is>
       </c>
     </row>
@@ -3075,36 +3308,27 @@
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Stato maggiore federale Protezione della popolazione</t>
-        </is>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>SMFP</t>
-        </is>
-      </c>
+          <t>Organo di condotta</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Nel caso in cui si delinea o si è verificato un evento di portata nazionale rilevante per la protezione della popolazione, lo SMFP assume i compiti seguenti (art. 4, cpv. 2 OSMFP):
-- assicura lo scambio di informazioni e il coordinamento con altri stati maggiori e organi della Confederazione e dei Cantoni, con i gestori di infrastrutture critiche e con i competenti organi all'estero;
-riunisce le situazioni settoriali e parziali per ottenere un quadro generale della situazione e ne effettua la valutazione.
-- elabora le basi decisionali all’attenzione del Consiglio federale, del dipartimento o dell’ufficio competente;
-- coordina le conoscenze degli esperti a livello federale;
-- coordina l'impiego delle risorse nazionali e internazionali.
-Lo SMFP si compone di una conferenza dei direttori, un elemento di pianificazione formato da esperti degli organi competenti e un elemento d'intervento e di supporto.</t>
-        </is>
-      </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>Competenza di protezione civile</t>
-        </is>
-      </c>
+          <t>Gli organi di condotta vengono istituiti dalle autorità competenti per lo svolgimento dei seguenti compiti: a - informare la popolazione in merito ai pericoli che la minacciano come pure alle possibilità e alle misure di protezione esistenti; b - avvertire, dare l’allarme e impartire alla popolazione istruzioni sul comportamento; c - assicurare le attività di condotta; d - coordinare i preparativi e gli interventi delle 
+ organizzazioni partner; e - garantire, tempestivamente e in funzione della situazione, la disponibilità operativa e il rinforzo con personale e materiale della protezione della popolazione in vista di un conflitto armato.</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
-      <c r="R42" t="inlineStr"/>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>Art. 4</t>
+        </is>
+      </c>
       <c r="S42" t="inlineStr"/>
       <c r="T42" t="inlineStr">
         <is>
-          <t>Elemento d'intervento e di supporto dello Stato maggiore federale Protezione della popolazione</t>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
         </is>
       </c>
       <c r="U42" t="inlineStr"/>
@@ -3115,16 +3339,16 @@
       </c>
       <c r="W42" t="inlineStr">
         <is>
-          <t>https://www.naz.ch/it/naz/eo.html</t>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
         </is>
       </c>
       <c r="X42" t="inlineStr"/>
       <c r="Y42" s="2" t="n">
-        <v>43656</v>
+        <v>43766</v>
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>ITCH00002</t>
+          <t>ITCH00011</t>
         </is>
       </c>
     </row>
@@ -3134,17 +3358,13 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Protezione civile</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>PC</t>
-        </is>
-      </c>
+          <t>Emergenza / Stato di emergenza / Evento emergenziale / Evento</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
+          <t>Indica l'insieme delle emergenze di tipo A, B e C così come definiti dall' Art. 7, comma 1 del DL 02/01/2018, n°1.</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -3155,12 +3375,12 @@
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Art 1, comma 1</t>
+          <t>Art 7, Comma 1</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=1&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=1&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0</t>
+          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=7&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=2&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -3185,30 +3405,26 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>Protezione civile</t>
+          <t>Stato di necessità</t>
         </is>
       </c>
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr">
         <is>
-          <t>La protezione civile protegge la popolazione, assiste le persone in cerca di protezione, protegge i beni culturali, sostiene gli organi di condotta e le altre organizzazioni partner nonché svolge lavori di ripristino e di pubblica utilità. Essa è un’organizzazione civile che opera singolarmente o in maniera coordinata, come organizzazione partner, all'interno della struttura svizzera di di protezione della popolazione.</t>
-        </is>
-      </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>Competenza di protezione civile</t>
-        </is>
-      </c>
+          <t>Si ha stato di necessità quando, a seguito di catastrofi, conflitti armati o altre situazioni d’emergenza che comportano un pericolo imminente per lo Stato, le persone o le cose, non sia più possibile garantire con i mezzi ordinari l’attività amministrativa o i servizi d’interesse pubblico e la protezione e l’assistenza delle persone e delle cose a livello cantonale, regionale o locale.</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr">
         <is>
-          <t>Art. 1</t>
+          <t>Art. 20</t>
         </is>
       </c>
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr">
         <is>
-          <t>Legge sulla protezione civile del 26 febbraio 2007</t>
+          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
         </is>
       </c>
       <c r="U43" t="inlineStr"/>
@@ -3219,20 +3435,20 @@
       </c>
       <c r="W43" t="inlineStr">
         <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/44</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
         </is>
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>Definizioni riorganizzate da Tommaso Sansone, Politecnico di Milano.</t>
+          <t>Per il lato italiano, definizione rielaborata da Tommaso Sansone a partire dall'art 7 del decreto di protezione civile 2-1-2018</t>
         </is>
       </c>
       <c r="Y43" s="2" t="n">
-        <v>43656</v>
+        <v>43412</v>
       </c>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>ITCH00003</t>
+          <t>ITCH00012</t>
         </is>
       </c>
     </row>
@@ -3253,31 +3469,26 @@
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr">
         <is>
-          <t>Comando della protezione civile</t>
+          <t>Impianto di protezione</t>
         </is>
       </c>
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Il comando della protezione civile è l’organo che dirige la protezione civile, ed è generalmente costituito dal comandante della protezione civile e dai suoi sostituti. I suoi compiti fondamentali sono i seguenti:
-- condurre gli interventi
-- condurre la protezione civile dal punto di vista organizzativo, amministrativo, del personale e del materiale
-- preparare, svolgere e valutare i corsi di ripetizione
-- assicurare l’efficienza operativa di costruzioni di protezione, materiale e infrastrutture per la diffusione dell’allarme
-- rappresentare le questioni della protezione civile presso le autorità, le organizzazioni partner, gli organi di condotta e la popolazione</t>
-        </is>
-      </c>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t>Competenza di protezione civile</t>
-        </is>
-      </c>
+          <t>Sono impianti di protezione: a - i posti di comando; b. gli impianti d’apprestamento; c - i centri sanitari protetti; d - gli ospedali protetti.</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr"/>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>Art. 50</t>
+        </is>
+      </c>
       <c r="S44" t="inlineStr"/>
       <c r="T44" t="inlineStr">
         <is>
-          <t>Il comando della protezione civile</t>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
         </is>
       </c>
       <c r="U44" t="inlineStr"/>
@@ -3288,16 +3499,16 @@
       </c>
       <c r="W44" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/it/zs/org/kdo.html</t>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
         </is>
       </c>
       <c r="X44" t="inlineStr"/>
       <c r="Y44" s="2" t="n">
-        <v>43656</v>
+        <v>43766</v>
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>ITCH00004</t>
+          <t>ITCH00013</t>
         </is>
       </c>
     </row>
@@ -3318,30 +3529,26 @@
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr">
         <is>
-          <t>Impianto di protezione per la protezione della popolazione</t>
+          <t>Costruzione di protezione</t>
         </is>
       </c>
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Si definiscono impianti di protezione i posti di comando, gli impianti d'apprestamento, i centri sanitari protetti e gli ospedali protetti. Essi vengono utilizzati soprattutto per garantire la condotta e l’operatività dei mezzi della protezione della popolazione.</t>
-        </is>
-      </c>
-      <c r="P45" t="inlineStr">
-        <is>
-          <t>Competenza di protezione civile</t>
-        </is>
-      </c>
+          <t>Le Costruzioni di protezione si distinguono in rifugi e impianti di protezione. Sono edifici che vengono costruiti o utilizzati ai fini di protezione della popolazione.</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr">
         <is>
-          <t>Impianti di protezione per la protezione della popolazione</t>
+          <t>Art. 45 e Art. 50</t>
         </is>
       </c>
       <c r="S45" t="inlineStr"/>
       <c r="T45" t="inlineStr">
         <is>
-          <t>Costruzioni di protezione</t>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
         </is>
       </c>
       <c r="U45" t="inlineStr"/>
@@ -3352,16 +3559,16 @@
       </c>
       <c r="W45" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/it/aufgabenbabs/schutzbauten.html</t>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
         </is>
       </c>
       <c r="X45" t="inlineStr"/>
       <c r="Y45" s="2" t="n">
-        <v>43657</v>
+        <v>43766</v>
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>ITCH00005</t>
+          <t>ITCH00014</t>
         </is>
       </c>
     </row>
@@ -3382,37 +3589,26 @@
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr">
         <is>
-          <t>Evento NBC</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>NBC</t>
-        </is>
-      </c>
+          <t>Rifugio</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Per evento NBC s'intende l'emissione illecita di sostanze nucleari (atomiche e radiologiche, N), biologiche (B) o chimiche (C). L'emissione può essere accidentale (incidente) o intenzionale (atto criminale o terroristico). Si distinguono i seguenti settori:
-- settore N: emissione di radiazioni ionizzanti e radioattività;
-- settore B: emissione di organismi patogeni (che causano malattie) o dei loro prodotti metabolici;
-- settore C: emissione di gas, liquidi o solidi tossici.</t>
-        </is>
-      </c>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t>Competenza di protezione civile</t>
-        </is>
-      </c>
+          <t>posto protetto di cui ogni abitante deve disporre e che sia raggiungibile in tempo utile dalla propria abitazione.</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr">
         <is>
-          <t>Definizione di „evento NBC“: emissione di sostanze pericolose</t>
+          <t>Art. 45</t>
         </is>
       </c>
       <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr">
         <is>
-          <t>La Protezione NBC</t>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
         </is>
       </c>
       <c r="U46" t="inlineStr"/>
@@ -3423,16 +3619,16 @@
       </c>
       <c r="W46" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/it/aufgabenbabs/abcschutz.html</t>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
         </is>
       </c>
       <c r="X46" t="inlineStr"/>
       <c r="Y46" s="2" t="n">
-        <v>43657</v>
+        <v>43766</v>
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>ITCH00006</t>
+          <t>ITCH00015</t>
         </is>
       </c>
     </row>
@@ -3440,67 +3636,63 @@
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Suscettibilità da Frana</t>
-        </is>
-      </c>
+      <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>La suscettibilità da frana è la probabilità che una frana avvenga in un territorio, sulla base delle condizioni locali. E’ una misura del grado in cui un territorio potrà essere interessato da frane, ossia una stima di “dove” le frane potranno accadere. La suscettibilità non considera la ricorrenza temporale, né la dimensione delle frane. In termini matematici, la suscettibilità da frana è comunemente espressa come la probabilità d’occorrenza spaziale di un dissesto, dato un insieme di condizioni territoriali e ambientali.</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Geologia e sismologia</t>
-        </is>
-      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>primo paragrafo</t>
-        </is>
-      </c>
+      <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>Modelli e carte di suscettibilità da frana</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>IRPI</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>IRPI CNR</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>http://www.irpi.cnr.it/focus/suscettibilita-da-frana/</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Addetto all'assistenza</t>
+        </is>
+      </c>
       <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr"/>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>milite impiegato, in funzione dell'evento o della situazione d'emergenza, per assistere persone in cerca di protezione (senzatetto, evacuati, ecc.) o aiutare i servizi della sanità pubblica (per es. in case per anziani). L'addetto all'assistenza deve disporre di buone competenze sociali e capacità organizzative.</t>
+        </is>
+      </c>
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr"/>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>pag 10</t>
+        </is>
+      </c>
       <c r="S47" t="inlineStr"/>
-      <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr"/>
-      <c r="V47" t="inlineStr"/>
-      <c r="W47" t="inlineStr"/>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>Il comando della protezione civile - Personale</t>
+        </is>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>Ufficio Federale della Protezione della Popolazione</t>
+        </is>
+      </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t>Confederazione Elvetica</t>
+        </is>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>https://www.babs.admin.ch/content/babs-internet/it/publikservice/downloads/unterlagen-ausbildung/_jcr_content/contentPar/accordion_1920886228/accordionItems/kommando_zivilschutz/accordionPar/downloadlist_copy/downloadItems/829_1459931125997.download/personal170191103it.pdf</t>
+        </is>
+      </c>
       <c r="X47" t="inlineStr"/>
       <c r="Y47" s="2" t="n">
-        <v>43731</v>
+        <v>43767</v>
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>ITCH00007</t>
+          <t>ITCH00016</t>
         </is>
       </c>
     </row>
@@ -3508,86 +3700,46 @@
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Vigili del fuoco</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>VVFF</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>In occasione degli eventi calamitosi, il Corpo nazionale dei vigili del fuoco opera gli interventi di soccorso tecnico indifferibili e urgenti: di ricerca e salvataggio delle persone e – ai fini della salvaguardia della pubblica incolumità – anche di messa in sicurezza dei luoghi, delle strutture e degli impianti.</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>Competenza di soccorso tecnico urgente; Competenza della Protezione Civile</t>
-        </is>
-      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>Art. 10</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=10&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=3&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0#art</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Presidenza Del Consiglio Dei Ministri</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>Gazzetta Ufficiale</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>https://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
-        </is>
-      </c>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr">
         <is>
-          <t>Pompieri</t>
+          <t>Assistente di stato maggiore</t>
         </is>
       </c>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr">
         <is>
-          <t>I pompieri sono responsabili di salvataggio e lotta contro i sinistri in generale, compresa la lotta antincendio e contro i sinistri ordinari. Intervengono anche in caso d’emissioni tossiche, fuoriuscite di carburanti e contaminazioni radioattive. Sono un mezzo di primo intervento.</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>Competenza di soccorso tecnico urgente; Competenza della Protezione Civile</t>
-        </is>
-      </c>
+          <t>milite impiegato per prestare aiuto alla condotta in seno all'organo di condotta o a favore dei partner ed istruito in materia di analisi della situazione e telematica. L'assistente di stato maggiore deve essere polivalente.</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr">
         <is>
-          <t>Art. 3</t>
+          <t>pag 9</t>
         </is>
       </c>
       <c r="S48" t="inlineStr"/>
       <c r="T48" t="inlineStr">
         <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
-        </is>
-      </c>
-      <c r="U48" t="inlineStr"/>
+          <t>Il comando della protezione civile - Personale</t>
+        </is>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>Ufficio Federale della Protezione della Popolazione</t>
+        </is>
+      </c>
       <c r="V48" t="inlineStr">
         <is>
           <t>Confederazione Elvetica</t>
@@ -3595,20 +3747,16 @@
       </c>
       <c r="W48" t="inlineStr">
         <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
-        </is>
-      </c>
-      <c r="X48" t="inlineStr">
-        <is>
-          <t>Per il lato italiano, definizione tratta dall'art 10 del codice di protezione civile del 2-1-2018, rielaborata da Tommaso Sansone.</t>
-        </is>
-      </c>
+          <t>https://www.babs.admin.ch/content/babs-internet/it/publikservice/downloads/unterlagen-ausbildung/_jcr_content/contentPar/accordion_1920886228/accordionItems/kommando_zivilschutz/accordionPar/downloadlist_copy/downloadItems/829_1459931125997.download/personal170191103it.pdf</t>
+        </is>
+      </c>
+      <c r="X48" t="inlineStr"/>
       <c r="Y48" s="2" t="n">
-        <v>43766</v>
+        <v>43767</v>
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>ITCH00009</t>
+          <t>ITCH00017</t>
         </is>
       </c>
     </row>
@@ -3616,107 +3764,67 @@
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Struttura operativa</t>
-        </is>
-      </c>
+      <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Oltre al Corpo nazionale dei vigili del fuoco, che opera quale componente fondamentale del Servizio nazionale della protezione civile, sono strutture operative nazionali: a) le Forze armate; b) le Forze di polizia; c) gli enti e istituti di ricerca di rilievo nazionale con finalità di protezione civile, anche organizzati come centri di competenza, l'Istituto nazionale di geofisica e vulcanologia e il Consiglio nazionale delle ricerche; d) le strutture del Servizio sanitario nazionale; e) il volontariato organizzato di protezione civile iscritto nell'elenco nazionale del volontariato di protezione civile, l'Associazione della Croce rossa italiana e il Corpo nazionale del soccorso alpino e speleologico; f) il Sistema nazionale per la protezione dell'ambiente; g) le strutture preposte alla gestione dei servizi meteorologici a livello nazionale.</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>Organizzazione degli Stati maggiori di condotta</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>OSMC</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>L’Organizzazione degli Stati maggiori di condotta (OSMC) è composta dai rappresentanti della Polizia cantonale, della Federazione cantonale ticinese corpi pompieri, della Federazione cantonale ticinese servizi autoambulanze, del Servizio della protezione civile cantonale, dei servizi tecnici e del Dipartimento delle istituzioni; ogni organizzazione designa il proprio rappresentante. A seconda delle necessità possono essere designati ulteriori responsabili per i servizi tecnici. L’OSMC è diretta dal rappresentante del Dipartimento.</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
         <is>
           <t>Competenza della Protezione Civile</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>Art. 13</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=13&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=3&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0#art</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>Presidenza Del Consiglio Dei Ministri</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>Gazzetta Ufficiale</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>https://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>Organizzazione partner</t>
-        </is>
-      </c>
-      <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>Sono organizzazioni partner quelle che collaborano alla protezione della popolazione: Polizia, pompieri, servizi della sanità pubblica, servizi tecnici, protezione civile.</t>
-        </is>
-      </c>
-      <c r="P49" t="inlineStr"/>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>confederazione elvetica</t>
-        </is>
-      </c>
+      <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr">
         <is>
-          <t>Art. 3</t>
+          <t>Art. 6</t>
         </is>
       </c>
       <c r="S49" t="inlineStr"/>
       <c r="T49" t="inlineStr">
         <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
-        </is>
-      </c>
-      <c r="U49" t="inlineStr">
-        <is>
-          <t>Confederazion elvetica</t>
-        </is>
-      </c>
+          <t>Regolamento sulla protezione della popolazione (RProtPop) (del 18 ottobre 2017)</t>
+        </is>
+      </c>
+      <c r="U49" t="inlineStr"/>
       <c r="V49" t="inlineStr">
         <is>
-          <t>Confederazione elvetica</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
       <c r="W49" t="inlineStr">
         <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
-        </is>
-      </c>
-      <c r="X49" t="inlineStr">
-        <is>
-          <t>strutture operative in italia e organizzazioni partner in svizzera hanno la stessa connotazione all'interno di un sistema di protezione della popolazione.</t>
-        </is>
-      </c>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/index/nuovafinestra/atto/49/volume/5%20SICUREZZA/numLegge/500.110</t>
+        </is>
+      </c>
+      <c r="X49" t="inlineStr"/>
       <c r="Y49" s="2" t="n">
-        <v>43766</v>
+        <v>43767</v>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>ITCH00010</t>
+          <t>ITCH00018</t>
         </is>
       </c>
     </row>
@@ -3737,30 +3845,36 @@
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Organo di condotta</t>
+          <t>Pioniere</t>
         </is>
       </c>
       <c r="N50" t="inlineStr"/>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Gli organi di condotta vengono istituiti dalle autorità competenti per lo svolgimento dei seguenti compiti: a - informare la popolazione in merito ai pericoli che la minacciano come pure alle possibilità e alle misure di protezione esistenti; b - avvertire, dare l’allarme e impartire alla popolazione istruzioni sul comportamento; c - assicurare le attività di condotta; d - coordinare i preparativi e gli interventi delle 
- organizzazioni partner; e - garantire, tempestivamente e in funzione della situazione, la disponibilità operativa e il rinforzo con personale e materiale della protezione della popolazione in vista di un conflitto armato.</t>
+          <t>milite impiegato soprattutto per assistere le organizzazioni
+partner nell'esecuzione dei lavori necessari per limitare o ripristinare i
+danni. Il pioniere deve presentare una corporatura robusta ed essere
+abile al lavoro manuale.</t>
         </is>
       </c>
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
       <c r="R50" t="inlineStr">
         <is>
-          <t>Art. 4</t>
+          <t>pag 10</t>
         </is>
       </c>
       <c r="S50" t="inlineStr"/>
       <c r="T50" t="inlineStr">
         <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
-        </is>
-      </c>
-      <c r="U50" t="inlineStr"/>
+          <t>Il comando della protezione civile - Personale</t>
+        </is>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>Ufficio Federale della Protezione della Popolazione</t>
+        </is>
+      </c>
       <c r="V50" t="inlineStr">
         <is>
           <t>Confederazione Elvetica</t>
@@ -3768,16 +3882,16 @@
       </c>
       <c r="W50" t="inlineStr">
         <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+          <t>https://www.babs.admin.ch/content/babs-internet/it/publikservice/downloads/unterlagen-ausbildung/_jcr_content/contentPar/accordion_1920886228/accordionItems/kommando_zivilschutz/accordionPar/downloadlist_copy/downloadItems/829_1459931125997.download/personal170191103it.pdf</t>
         </is>
       </c>
       <c r="X50" t="inlineStr"/>
       <c r="Y50" s="2" t="n">
-        <v>43766</v>
+        <v>43767</v>
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>ITCH00011</t>
+          <t>ITCH00019</t>
         </is>
       </c>
     </row>
@@ -3785,73 +3899,41 @@
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Emergenza / Stato di emergenza / Evento emergenziale / Evento</t>
-        </is>
-      </c>
+      <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Indica l'insieme delle emergenze di tipo A, B e C così come definiti dall' Art. 7, comma 1 del DL 02/01/2018, n°1.</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Competenza di protezione civile</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Tommaso Sansone</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>Art 7, Comma 1</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=7&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=2&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>Presidenza Del Consiglio Dei Ministri</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>Gazzetta Ufficiale</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>http://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
-        </is>
-      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
       <c r="M51" t="inlineStr">
         <is>
-          <t>Stato di necessità</t>
-        </is>
-      </c>
-      <c r="N51" t="inlineStr"/>
+          <t>Stato maggiore cantonale di condotta</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>SMCC</t>
+        </is>
+      </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Si ha stato di necessità quando, a seguito di catastrofi, conflitti armati o altre situazioni d’emergenza che comportano un pericolo imminente per lo Stato, le persone o le cose, non sia più possibile garantire con i mezzi ordinari l’attività amministrativa o i servizi d’interesse pubblico e la protezione e l’assistenza delle persone e delle cose a livello cantonale, regionale o locale.</t>
-        </is>
-      </c>
-      <c r="P51" t="inlineStr"/>
+          <t>Lo SMCC è l’organo cantonale di condotta del Consiglio di Stato, che ne definisce la composizione, l’organizzazione e il funzionamento. Esso elabora le basi decisionali per il Consiglio di Stato, lo coadiuva nelle funzioni di direzione e coordinamento ed esegue le sue decisioni. Esso è competente quando le circostanze lo esigono, per predisporre e coordinare, in collaborazione con le autorità locali, le necessarie misure d’urgenza e di assistenza e condurne l’attuazione. La sua attivazione è decisa dal Comandante della Polizia cantonale; in caso di impedimento di questo e in successione, dal suo sostituto o dall’ufficiale di picchetto della Polizia cantonale.</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>Competenza della Protezione Civile</t>
+        </is>
+      </c>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr">
         <is>
-          <t>Art. 20</t>
+          <t>Art. 10</t>
         </is>
       </c>
       <c r="S51" t="inlineStr"/>
@@ -3871,17 +3953,13 @@
           <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
         </is>
       </c>
-      <c r="X51" t="inlineStr">
-        <is>
-          <t>Per il lato italiano, definizione rielaborata da Tommaso Sansone a partire dall'art 7 del decreto di protezione civile 2-1-2018</t>
-        </is>
-      </c>
+      <c r="X51" t="inlineStr"/>
       <c r="Y51" s="2" t="n">
-        <v>43412</v>
+        <v>43767</v>
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>ITCH00012</t>
+          <t>ITCH00020</t>
         </is>
       </c>
     </row>
@@ -3902,46 +3980,30 @@
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr">
         <is>
-          <t>Impianto di protezione</t>
+          <t>Sistema d’allarme acqua</t>
         </is>
       </c>
       <c r="N52" t="inlineStr"/>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Sono impianti di protezione: a - i posti di comando; b. gli impianti d’apprestamento; c - i centri sanitari protetti; d - gli ospedali protetti.</t>
+          <t>Sistema di allertamento per eventi di tipo idrometeorologico.</t>
         </is>
       </c>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>Art. 50</t>
-        </is>
-      </c>
+      <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr"/>
-      <c r="T52" t="inlineStr">
-        <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
-        </is>
-      </c>
+      <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr"/>
-      <c r="V52" t="inlineStr">
-        <is>
-          <t>Confederazione Elvetica</t>
-        </is>
-      </c>
-      <c r="W52" t="inlineStr">
-        <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
-        </is>
-      </c>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr"/>
       <c r="Y52" s="2" t="n">
         <v>43766</v>
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>ITCH00013</t>
+          <t>ITCH00021</t>
         </is>
       </c>
     </row>
@@ -3962,26 +4024,22 @@
       <c r="L53" t="inlineStr"/>
       <c r="M53" t="inlineStr">
         <is>
-          <t>Costruzione di protezione</t>
+          <t>Allarme acqua</t>
         </is>
       </c>
       <c r="N53" t="inlineStr"/>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Le Costruzioni di protezione si distinguono in rifugi e impianti di protezione. Sono edifici che vengono costruiti o utilizzati ai fini di protezione della popolazione.</t>
+          <t>Il segnale d'allarme acqua viene emesso esclusivamente nelle regioni minacciate a valle di impianti d'accumulazione. Le sirene emettono dodici suoni continui e gravi in sequenze di 20 secondi e a intervalli di 10 secondi. L’allarme acqua esorta la popolazione ad abbandonare immediatamente la regione minacciata.</t>
         </is>
       </c>
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>Art. 45 e Art. 50</t>
-        </is>
-      </c>
+      <c r="R53" t="inlineStr"/>
       <c r="S53" t="inlineStr"/>
       <c r="T53" t="inlineStr">
         <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
+          <t>Segnali di allarme in Svizzera</t>
         </is>
       </c>
       <c r="U53" t="inlineStr"/>
@@ -3992,16 +4050,16 @@
       </c>
       <c r="W53" t="inlineStr">
         <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+          <t>https://www.ch.ch/it/allarme-sirene/</t>
         </is>
       </c>
       <c r="X53" t="inlineStr"/>
       <c r="Y53" s="2" t="n">
-        <v>43766</v>
+        <v>43767</v>
       </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>ITCH00014</t>
+          <t>ITCH00022</t>
         </is>
       </c>
     </row>
@@ -4022,46 +4080,54 @@
       <c r="L54" t="inlineStr"/>
       <c r="M54" t="inlineStr">
         <is>
-          <t>Rifugio</t>
-        </is>
-      </c>
-      <c r="N54" t="inlineStr"/>
+          <t>Stato maggiore regionale di condotta</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>SMRC</t>
+        </is>
+      </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>posto protetto di cui ogni abitante deve disporre e che sia raggiungibile in tempo utile dalla propria abitazione.</t>
-        </is>
-      </c>
-      <c r="P54" t="inlineStr"/>
+          <t>Lo SMRC è un organo di condotta che permette la coordinazione di più SMEPI attivi nella medesima regione. La costituzione di uno SMRC può essere ordinata o autorizzata dal Comandante dello SMCC. Esso è di norma condotto da un ufficiale della Polizia cantonale.</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>Competenza della Protezione Civile</t>
+        </is>
+      </c>
       <c r="Q54" t="inlineStr"/>
       <c r="R54" t="inlineStr">
         <is>
-          <t>Art. 45</t>
+          <t>Art. 11</t>
         </is>
       </c>
       <c r="S54" t="inlineStr"/>
       <c r="T54" t="inlineStr">
         <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
+          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
         </is>
       </c>
       <c r="U54" t="inlineStr"/>
       <c r="V54" t="inlineStr">
         <is>
-          <t>Confederazione Elvetica</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
       <c r="W54" t="inlineStr">
         <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
         </is>
       </c>
       <c r="X54" t="inlineStr"/>
       <c r="Y54" s="2" t="n">
-        <v>43766</v>
+        <v>43767</v>
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>ITCH00015</t>
+          <t>ITCH00023</t>
         </is>
       </c>
     </row>
@@ -4082,41 +4148,41 @@
       <c r="L55" t="inlineStr"/>
       <c r="M55" t="inlineStr">
         <is>
-          <t>Addetto all'assistenza</t>
-        </is>
-      </c>
-      <c r="N55" t="inlineStr"/>
+          <t>Stato maggiore enti di primo intervento</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>SMEPI</t>
+        </is>
+      </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>milite impiegato, in funzione dell'evento o della situazione d'emergenza, per assistere persone in cerca di protezione (senzatetto, evacuati, ecc.) o aiutare i servizi della sanità pubblica (per es. in case per anziani). L'addetto all'assistenza deve disporre di buone competenze sociali e capacità organizzative.</t>
+          <t>Lo SMEPI coordina l’intervento dei primi enti mobilitati, di regola polizia, pompieri e servizi d’autoambulanza. Esso è condotto, di principio, dalla Polizia cantonale.</t>
         </is>
       </c>
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="inlineStr">
         <is>
-          <t>pag 10</t>
+          <t>Art. 12</t>
         </is>
       </c>
       <c r="S55" t="inlineStr"/>
       <c r="T55" t="inlineStr">
         <is>
-          <t>Il comando della protezione civile - Personale</t>
-        </is>
-      </c>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>Ufficio Federale della Protezione della Popolazione</t>
-        </is>
-      </c>
+          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
+        </is>
+      </c>
+      <c r="U55" t="inlineStr"/>
       <c r="V55" t="inlineStr">
         <is>
-          <t>Confederazione Elvetica</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
       <c r="W55" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/content/babs-internet/it/publikservice/downloads/unterlagen-ausbildung/_jcr_content/contentPar/accordion_1920886228/accordionItems/kommando_zivilschutz/accordionPar/downloadlist_copy/downloadItems/829_1459931125997.download/personal170191103it.pdf</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
         </is>
       </c>
       <c r="X55" t="inlineStr"/>
@@ -4125,7 +4191,7 @@
       </c>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>ITCH00016</t>
+          <t>ITCH00024</t>
         </is>
       </c>
     </row>
@@ -4133,63 +4199,114 @@
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Protezione civile</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Competenza di protezione civile</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
-      <c r="J56" t="inlineStr"/>
-      <c r="K56" t="inlineStr"/>
-      <c r="L56" t="inlineStr"/>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Art 1, comma 1</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=1&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=1&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Presidenza Del Consiglio Dei Ministri</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Gazzetta Ufficiale</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>http://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
+        </is>
+      </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>Assistente di stato maggiore</t>
+          <t>Protezione della popolazione</t>
         </is>
       </c>
       <c r="N56" t="inlineStr"/>
       <c r="O56" t="inlineStr">
         <is>
-          <t>milite impiegato per prestare aiuto alla condotta in seno all'organo di condotta o a favore dei partner ed istruito in materia di analisi della situazione e telematica. L'assistente di stato maggiore deve essere polivalente.</t>
-        </is>
-      </c>
-      <c r="P56" t="inlineStr"/>
+          <t>Il servizio della protezione della popolazione si occupa prevalentemente dei preparativi per i casi di emergenza e di catastrofe.
+Assicura la collaborazione con i servizi delle Amministrazioni: federale, cantonale e comunali direttamente collegate con i temi trattati dal servizio e si occupa della coordinazione fra i partner del concetto “protezione della popolazione” (polizia cantonale, Federazione cantonale ticinese dei Corpi Pompieri, Federazione cantonale ticinese dei Servizi autoambulanze, organizzazioni regionali di protezione civile, servizi tecnici cantonali, servizi dello Stato Maggiore cantonale di catastrofe, ecc…).
+Per il tramite di esercitazioni teoriche e pratiche, approfondisce con le istanze militari, la collaborazione civile-militare.</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>Competenza della Protezione Civile</t>
+        </is>
+      </c>
       <c r="Q56" t="inlineStr"/>
       <c r="R56" t="inlineStr">
         <is>
-          <t>pag 9</t>
+          <t>Presentazione</t>
         </is>
       </c>
       <c r="S56" t="inlineStr"/>
       <c r="T56" t="inlineStr">
         <is>
-          <t>Il comando della protezione civile - Personale</t>
+          <t>Servizio della protezione della popolazione</t>
         </is>
       </c>
       <c r="U56" t="inlineStr">
         <is>
-          <t>Ufficio Federale della Protezione della Popolazione</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>Confederazione Elvetica</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
       <c r="W56" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/content/babs-internet/it/publikservice/downloads/unterlagen-ausbildung/_jcr_content/contentPar/accordion_1920886228/accordionItems/kommando_zivilschutz/accordionPar/downloadlist_copy/downloadItems/829_1459931125997.download/personal170191103it.pdf</t>
-        </is>
-      </c>
-      <c r="X56" t="inlineStr"/>
+          <t>https://www4.ti.ch/di/smpp/chi-siamo/servizio-della-protezione-della-popolazione/</t>
+        </is>
+      </c>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>Il significato italiano di protezione civile coincide a livello di strutture con io significato svizzero di protezione della popolazione.
+Definizioni riorganizzate da Tommaso Sansone, Politecnico di Milano.</t>
+        </is>
+      </c>
       <c r="Y56" s="2" t="n">
-        <v>43767</v>
+        <v>43815</v>
       </c>
       <c r="Z56" t="inlineStr">
         <is>
-          <t>ITCH00017</t>
+          <t>ITCH00025</t>
         </is>
       </c>
     </row>
@@ -4197,67 +4314,55 @@
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B57" t="inlineStr"/>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Dipartimento della protezione civile</t>
+        </is>
+      </c>
       <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Il Dipartimento della protezione civile è una struttura della Presidenza del Consiglio dei Ministri. Il Dipartimento, operando in stretto raccordo con le Regioni e le Province autonome, si occupa di tutte le attività volte alla previsione e alla prevenzione dei rischi, al soccorso e all’assistenza delle popolazioni colpite da calamità, al contrasto e al superamento dell’emergenza.</t>
+        </is>
+      </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Dipartimento</t>
+        </is>
+      </c>
       <c r="J57" t="inlineStr"/>
-      <c r="K57" t="inlineStr"/>
-      <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>Organizzazione degli Stati maggiori di condotta</t>
-        </is>
-      </c>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t>OSMC</t>
-        </is>
-      </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>L’Organizzazione degli Stati maggiori di condotta (OSMC) è composta dai rappresentanti della Polizia cantonale, della Federazione cantonale ticinese corpi pompieri, della Federazione cantonale ticinese servizi autoambulanze, del Servizio della protezione civile cantonale, dei servizi tecnici e del Dipartimento delle istituzioni; ogni organizzazione designa il proprio rappresentante. A seconda delle necessità possono essere designati ulteriori responsabili per i servizi tecnici. L’OSMC è diretta dal rappresentante del Dipartimento.</t>
-        </is>
-      </c>
-      <c r="P57" t="inlineStr">
-        <is>
-          <t>Competenza della Protezione Civile</t>
-        </is>
-      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Dipartimento della protezione civile</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>http://www.protezionecivile.gov.it/dipartimento</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
       <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr">
-        <is>
-          <t>Art. 6</t>
-        </is>
-      </c>
+      <c r="R57" t="inlineStr"/>
       <c r="S57" t="inlineStr"/>
-      <c r="T57" t="inlineStr">
-        <is>
-          <t>Regolamento sulla protezione della popolazione (RProtPop) (del 18 ottobre 2017)</t>
-        </is>
-      </c>
+      <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr"/>
-      <c r="V57" t="inlineStr">
-        <is>
-          <t>Repubblica e Cantone Ticino</t>
-        </is>
-      </c>
-      <c r="W57" t="inlineStr">
-        <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/index/nuovafinestra/atto/49/volume/5%20SICUREZZA/numLegge/500.110</t>
-        </is>
-      </c>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
       <c r="X57" t="inlineStr"/>
       <c r="Y57" s="2" t="n">
-        <v>43767</v>
+        <v>43817</v>
       </c>
       <c r="Z57" t="inlineStr">
         <is>
-          <t>ITCH00018</t>
+          <t>ITCH00026</t>
         </is>
       </c>
     </row>
@@ -4267,10 +4372,22 @@
       </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr"/>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>La legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002 può essere considerata come la più importante legge dello stato svizzero in materia di protezione della protezione della popolazione, che costituisce quadro normativo di riferimento per altre leggi federali e cantonali in materia di protezione della popolazione. Essa disciplina principalmente due ambiti: - la collaborazione tra Confederazione e Cantoni nella protezione della popolazione. - il ruolo e i doveri degli organi e dei corpi della protezione della popolazione.</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Normativa</t>
+        </is>
+      </c>
       <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr"/>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Normativa nazionale: Legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002</t>
+        </is>
+      </c>
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr"/>
@@ -4278,53 +4395,34 @@
       <c r="L58" t="inlineStr"/>
       <c r="M58" t="inlineStr">
         <is>
-          <t>Pioniere</t>
-        </is>
-      </c>
-      <c r="N58" t="inlineStr"/>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>milite impiegato soprattutto per assistere le organizzazioni
-partner nell'esecuzione dei lavori necessari per limitare o ripristinare i
-danni. Il pioniere deve presentare una corporatura robusta ed essere
-abile al lavoro manuale.</t>
-        </is>
-      </c>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>LPPC</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr"/>
       <c r="P58" t="inlineStr"/>
       <c r="Q58" t="inlineStr"/>
-      <c r="R58" t="inlineStr">
-        <is>
-          <t>pag 10</t>
-        </is>
-      </c>
+      <c r="R58" t="inlineStr"/>
       <c r="S58" t="inlineStr"/>
-      <c r="T58" t="inlineStr">
-        <is>
-          <t>Il comando della protezione civile - Personale</t>
-        </is>
-      </c>
-      <c r="U58" t="inlineStr">
-        <is>
-          <t>Ufficio Federale della Protezione della Popolazione</t>
-        </is>
-      </c>
-      <c r="V58" t="inlineStr">
-        <is>
-          <t>Confederazione Elvetica</t>
-        </is>
-      </c>
-      <c r="W58" t="inlineStr">
-        <is>
-          <t>https://www.babs.admin.ch/content/babs-internet/it/publikservice/downloads/unterlagen-ausbildung/_jcr_content/contentPar/accordion_1920886228/accordionItems/kommando_zivilschutz/accordionPar/downloadlist_copy/downloadItems/829_1459931125997.download/personal170191103it.pdf</t>
-        </is>
-      </c>
-      <c r="X58" t="inlineStr"/>
+      <c r="T58" t="inlineStr"/>
+      <c r="U58" t="inlineStr"/>
+      <c r="V58" t="inlineStr"/>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>definizione lato italiano, oggetto lato svizzero</t>
+        </is>
+      </c>
       <c r="Y58" s="2" t="n">
-        <v>43767</v>
+        <v>43780</v>
       </c>
       <c r="Z58" t="inlineStr">
         <is>
-          <t>ITCH00019</t>
+          <t>ITCH00027</t>
         </is>
       </c>
     </row>
@@ -4332,30 +4430,51 @@
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B59" t="inlineStr"/>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Volontario di protezione civile</t>
+        </is>
+      </c>
       <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Il decreto legislativo n. 1 del 2018, Codice della Protezioone Civile, include il volontariato organizzato di protezione civile iscritto nell'elenco nazionale del volontariato di protezione civile tra le strutture operative del Servizio nazionale. Il volontariato si integra con gli altri livelli territoriali di intervento previsti nell'organizzazione del sistema nazionale della protezione civile, in base al principio della sussidiarietà verticale. È inoltre attore del sistema e del proprio territorio: protegge la comunità in collaborazione con le istituzioni, in base al principio della sussidiarietà orizzontale.</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Competenza della Protezione Civile</t>
+        </is>
+      </c>
       <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Home &gt; Servizio Nazionale &gt; Strutture operative &gt; Volontariato</t>
+        </is>
+      </c>
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr"/>
-      <c r="K59" t="inlineStr"/>
-      <c r="L59" t="inlineStr"/>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Dipartimento della protezione civile</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>http://www.protezionecivile.gov.it/servizio-nazionale/strutture-operative/volontariato</t>
+        </is>
+      </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>Stato maggiore cantonale di condotta</t>
-        </is>
-      </c>
-      <c r="N59" t="inlineStr">
-        <is>
-          <t>SMCC</t>
-        </is>
-      </c>
+          <t>Volontario di protezione civile</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr"/>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Lo SMCC è l’organo cantonale di condotta del Consiglio di Stato, che ne definisce la composizione, l’organizzazione e il funzionamento. Esso elabora le basi decisionali per il Consiglio di Stato, lo coadiuva nelle funzioni di direzione e coordinamento ed esegue le sue decisioni. Esso è competente quando le circostanze lo esigono, per predisporre e coordinare, in collaborazione con le autorità locali, le necessarie misure d’urgenza e di assistenza e condurne l’attuazione. La sua attivazione è decisa dal Comandante della Polizia cantonale; in caso di impedimento di questo e in successione, dal suo sostituto o dall’ufficiale di picchetto della Polizia cantonale.</t>
+          <t>La legge LPPC 2002 stabilisce che possono prestare volontariamente servizio di protezione civile: a. gli uomini prosciolti dall’obbligo di prestare servizio nella protezione civile; b. gli uomini soggetti all’obbligo militare prosciolti dall’obbligo di prestare servizio militare o civile; c. gli uomini prosciolti dall’obbligo di prestare servizio militare o civile; d. le cittadine svizzere, a partire dall’anno in cui compiono i 20 anni; e. gli stranieri domiciliati in Svizzera, a partire dall’anno in cui compiono i 20 anni. Bisogna porre attenzione al fatto che secondo la stessa legge, l’unica differenza tra un milite e un volontario (entrambi di protezione civile) è il fatto che i volontari sono prosciolti dall’obbligo di prestare servizio su domanda. Infatti, per il resto, militi e volontari hanno gli stessi diritti e doveri. 
+I diritti dei militi sono essenzialmente quattro: soldo e vitto, alloggio, trasporto gratuiti, cui si aggiungono alcune agevolazioni fiscali e indennità.</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4366,24 +4485,16 @@
       <c r="Q59" t="inlineStr"/>
       <c r="R59" t="inlineStr">
         <is>
-          <t>Art. 10</t>
+          <t>Normativa nazionale: Legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002</t>
         </is>
       </c>
       <c r="S59" t="inlineStr"/>
-      <c r="T59" t="inlineStr">
-        <is>
-          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
-        </is>
-      </c>
+      <c r="T59" t="inlineStr"/>
       <c r="U59" t="inlineStr"/>
-      <c r="V59" t="inlineStr">
-        <is>
-          <t>Repubblica e Cantone Ticino</t>
-        </is>
-      </c>
+      <c r="V59" t="inlineStr"/>
       <c r="W59" t="inlineStr">
         <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
         </is>
       </c>
       <c r="X59" t="inlineStr"/>
@@ -4392,7 +4503,7 @@
       </c>
       <c r="Z59" t="inlineStr">
         <is>
-          <t>ITCH00020</t>
+          <t>ITCH00028</t>
         </is>
       </c>
     </row>
@@ -4413,34 +4524,51 @@
       <c r="L60" t="inlineStr"/>
       <c r="M60" t="inlineStr">
         <is>
-          <t>Sistema d’allarme acqua</t>
+          <t>Consiglio di stato</t>
         </is>
       </c>
       <c r="N60" t="inlineStr"/>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Sistema di allertamento per eventi di tipo idrometeorologico.</t>
+          <t>Il Consiglio di Stato è l’autorità competente per: a) assicurare la condotta, l’intervento e il coordinamento delle organizzazioni partner; b) assicurare l’istruzione e la formazione, anche degli organi di condotta locali; c) promuovere l’aiuto intercomunale, così come la cooperazione intercantonale e
+transfrontaliera; d) esercitare le altre funzioni attribuitegli dalla presente legge.</t>
         </is>
       </c>
       <c r="P60" t="inlineStr"/>
-      <c r="Q60" t="inlineStr">
-        <is>
-          <t>Tommaso Sansone</t>
-        </is>
-      </c>
-      <c r="R60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>Art. 7</t>
+        </is>
+      </c>
       <c r="S60" t="inlineStr"/>
-      <c r="T60" t="inlineStr"/>
-      <c r="U60" t="inlineStr"/>
-      <c r="V60" t="inlineStr"/>
-      <c r="W60" t="inlineStr"/>
+      <c r="T60" t="inlineStr">
+        <is>
+          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
+        </is>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>Ufficio Federale della Protezione della Popolazione</t>
+        </is>
+      </c>
+      <c r="V60" t="inlineStr">
+        <is>
+          <t>Repubblica e Cantone Ticino</t>
+        </is>
+      </c>
+      <c r="W60" t="inlineStr">
+        <is>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/pdfatto/atto/48</t>
+        </is>
+      </c>
       <c r="X60" t="inlineStr"/>
       <c r="Y60" s="2" t="n">
-        <v>43766</v>
+        <v>43817</v>
       </c>
       <c r="Z60" t="inlineStr">
         <is>
-          <t>ITCH00021</t>
+          <t>ITCH00029</t>
         </is>
       </c>
     </row>
@@ -4461,42 +4589,35 @@
       <c r="L61" t="inlineStr"/>
       <c r="M61" t="inlineStr">
         <is>
-          <t>Allarme acqua</t>
+          <t>Milite</t>
         </is>
       </c>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Il segnale d'allarme acqua viene emesso esclusivamente nelle regioni minacciate a valle di impianti d'accumulazione. Le sirene emettono dodici suoni continui e gravi in sequenze di 20 secondi e a intervalli di 10 secondi. L’allarme acqua esorta la popolazione ad abbandonare immediatamente la regione minacciata.</t>
+          <t>I militi svizzeri sono reclutati dall’esercito e dalla protezione civile e di norma vengono assegnati al loro cantone di domicilio, oppure ad altri cantoni, se deciso dal cantone di domicilio, cui comunque spetta la scelta. I militi, oltre ad essere arruolati in maniera ordinaria, possono essere incorporati nel personale di riserva. Se un milite entra a far parte del personale di riserva non deve essere necessariamente formato e non ha diritto a prestare servizio di protezione civile.
+Una volta reclutati e addestrasti, i militi possono essere chiamati a prestare servizio dal consiglio federale o dal cantone cui sono assegnati. Il Consiglio federale e il cantone di assegnamento possono chiamare in servizio i militi di protezione civile in caso di catastrofi e situazioni d’emergenza che colpiscono uno o più Cantoni, oppure le zone limitrofe di Paesi confinanti, oppure in caso di conflitto armato. I militi possono inoltre essere mobilitati anche in assenza di emergenza per svolgere dei lavori di ripristino di pubblica utilità. In quest’ultimo caso però, esistono dei limiti al potere di convocazione esercitato dalle autorità sui militi .</t>
         </is>
       </c>
       <c r="P61" t="inlineStr"/>
       <c r="Q61" t="inlineStr"/>
       <c r="R61" t="inlineStr"/>
       <c r="S61" t="inlineStr"/>
-      <c r="T61" t="inlineStr">
-        <is>
-          <t>Segnali di allarme in Svizzera</t>
-        </is>
-      </c>
+      <c r="T61" t="inlineStr"/>
       <c r="U61" t="inlineStr"/>
-      <c r="V61" t="inlineStr">
-        <is>
-          <t>Confederazione Elvetica</t>
-        </is>
-      </c>
-      <c r="W61" t="inlineStr">
-        <is>
-          <t>https://www.ch.ch/it/allarme-sirene/</t>
-        </is>
-      </c>
-      <c r="X61" t="inlineStr"/>
+      <c r="V61" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>Definizione italiana, oggetto svizzero. definizione rielaborata nel report wp2 di Gestisco, paragrafo Normativa nazionale: Legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002</t>
+        </is>
+      </c>
       <c r="Y61" s="2" t="n">
-        <v>43767</v>
+        <v>43766</v>
       </c>
       <c r="Z61" t="inlineStr">
         <is>
-          <t>ITCH00022</t>
+          <t>ITCH00030</t>
         </is>
       </c>
     </row>
@@ -4517,54 +4638,43 @@
       <c r="L62" t="inlineStr"/>
       <c r="M62" t="inlineStr">
         <is>
-          <t>Stato maggiore regionale di condotta</t>
+          <t>Legge sulla protezione della popolazione del 26 febbraio 2007</t>
         </is>
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>SMRC</t>
+          <t>LProtPop</t>
         </is>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Lo SMRC è un organo di condotta che permette la coordinazione di più SMEPI attivi nella medesima regione. La costituzione di uno SMRC può essere ordinata o autorizzata dal Comandante dello SMCC. Esso è di norma condotto da un ufficiale della Polizia cantonale.</t>
-        </is>
-      </c>
-      <c r="P62" t="inlineStr">
-        <is>
-          <t>Competenza della Protezione Civile</t>
-        </is>
-      </c>
+          <t>La legge cantonale del 26 febbraio 2007 è legge di maggior riferimento del Canton Ticino in materia di protezione della popolazione.
+Essa riprende alcuni argomenti già sanciti dalla legge federale LPPC del 2002, approfondisce la struttura e i compiti di alcuni organi di protezione della popolazione cantonali, quali gli organi di condotta, e descrive il concetto di stato di necessità a livello cantonale.</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr"/>
       <c r="Q62" t="inlineStr"/>
       <c r="R62" t="inlineStr">
         <is>
-          <t>Art. 11</t>
+          <t>Normativa cantonale: Legge sulla protezione della popolazione (LProtPop) del 26 febbraio 2007</t>
         </is>
       </c>
       <c r="S62" t="inlineStr"/>
-      <c r="T62" t="inlineStr">
-        <is>
-          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
-        </is>
-      </c>
+      <c r="T62" t="inlineStr"/>
       <c r="U62" t="inlineStr"/>
-      <c r="V62" t="inlineStr">
-        <is>
-          <t>Repubblica e Cantone Ticino</t>
-        </is>
-      </c>
-      <c r="W62" t="inlineStr">
-        <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
-        </is>
-      </c>
-      <c r="X62" t="inlineStr"/>
+      <c r="V62" t="inlineStr"/>
+      <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>definizione italiana, oggetto svizzero</t>
+        </is>
+      </c>
       <c r="Y62" s="2" t="n">
-        <v>43767</v>
+        <v>43817</v>
       </c>
       <c r="Z62" t="inlineStr">
         <is>
-          <t>ITCH00023</t>
+          <t>ITCH00031</t>
         </is>
       </c>
     </row>
@@ -4585,50 +4695,51 @@
       <c r="L63" t="inlineStr"/>
       <c r="M63" t="inlineStr">
         <is>
-          <t>Stato maggiore enti di primo intervento</t>
+          <t>sezione del militare e della protezione della popolazione</t>
         </is>
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>SMEPI</t>
+          <t>SMPP</t>
         </is>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Lo SMEPI coordina l’intervento dei primi enti mobilitati, di regola polizia, pompieri e servizi d’autoambulanza. Esso è condotto, di principio, dalla Polizia cantonale.</t>
+          <t>La Sezione è articolata in cinque servizi con distinte aree di competenza: il Servizio amministrativo, il Servizio degli affari militari e del comando di circondario, il Servizio della protezione civile, il Servizio costruzioni di protezione civile e il Servizio della protezione della popolazione. 
+Il servizio amministrativo centralizzato della sezione si occupa di fornire le prime informazioni all’utenza e di smistarle ai vari servizi di competenza. Altri compiti specifici sono la contabilità, la corrispondenza e il supporto logistico per tutta la sezione. 
+Il Servizio degli affari militari e comando di circondario si occupa delle pratiche amministrative legate ai servizi d’istruzione dei militi domiciliati in Ticino come pure degli obblighi fuori servizio (tiro obbligatorio, obbligo di notifica), tiene il controllo dei dati di servizio e di quelli personali dei militi con la collaborazione degli uffici di controllo abitanti dei comuni. 
+Il Servizio della protezione civile, unitamente al Centro istruzione della protezione civile di Rivera, assicura l'applicazione delle norme federali e cantonali di protezione civile nelle regioni e nei comuni, cura le diverse pianificazioni (allarmi, approvvigionamenti,...) e l'istruzione dei militi astretti.
+Il Servizio costruzioni si occupa della pianificazione e gestione dei posti protetti, come pure della realizzazione delle costruzioni protette (rifugi, impianti regionali).
+Il servizio della protezione della popolazione si occupa prevalentemente dei preparativi per i casi di emergenza e di catastrofe.</t>
         </is>
       </c>
       <c r="P63" t="inlineStr"/>
       <c r="Q63" t="inlineStr"/>
-      <c r="R63" t="inlineStr">
-        <is>
-          <t>Art. 12</t>
-        </is>
-      </c>
+      <c r="R63" t="inlineStr"/>
       <c r="S63" t="inlineStr"/>
       <c r="T63" t="inlineStr">
         <is>
-          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
+          <t>Chi siamo</t>
         </is>
       </c>
       <c r="U63" t="inlineStr"/>
       <c r="V63" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Repubblica e Canton Ticino</t>
         </is>
       </c>
       <c r="W63" t="inlineStr">
         <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
+          <t>https://www4.ti.ch/di/smpp/chi-siamo/presentazione/</t>
         </is>
       </c>
       <c r="X63" t="inlineStr"/>
       <c r="Y63" s="2" t="n">
-        <v>43767</v>
+        <v>43845</v>
       </c>
       <c r="Z63" t="inlineStr">
         <is>
-          <t>ITCH00024</t>
+          <t>ITCH00032</t>
         </is>
       </c>
     </row>
@@ -4638,112 +4749,57 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Protezione civile</t>
+          <t>Sala Operativa Regionale dell'Emergenza Urgenza</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>PC</t>
+          <t>SOREU</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>Competenza di protezione civile</t>
-        </is>
-      </c>
+          <t>Le SOREU hanno valenza interprovinciale: gestiscono le chiamate di soccorso sanitario con l'invio dei mezzi più appropriati fino al completamento del soccorso e/o all'eventuale affidamento del paziente alle strutture ospedaliere più idonee. Le SOREU operano tramite le dotazioni tecnologiche assegnate da AREU che permettono loro una costante interconnessione con i Call Center NUE 112 di riferimento, con i mezzi di soccorso delle AAT della propria area di competenza e con i Call Center sanitari specialistici, in modo da ottimizzare i tempi di risposta e intervento.</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Art 1, comma 1</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>https://www.gazzettaufficiale.it/atto/serie_generale/caricaArticolo?art.progressivo=0&amp;art.idArticolo=1&amp;art.versione=1&amp;art.codiceRedazionale=18G00011&amp;art.dataPubblicazioneGazzetta=2018-01-22&amp;art.idGruppo=1&amp;art.idSottoArticolo1=10&amp;art.idSottoArticolo=1&amp;art.flagTipoArticolo=0</t>
-        </is>
-      </c>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr">
         <is>
-          <t>Decreto Legislativo 2 Gennaio 2018, N. 1, Codice Della Protezione Civile. (18G00011)</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>Presidenza Del Consiglio Dei Ministri</t>
-        </is>
-      </c>
+          <t>Le SOREU</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr"/>
       <c r="K64" t="inlineStr">
         <is>
-          <t>Gazzetta Ufficiale</t>
+          <t>Areu Lombardia</t>
         </is>
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>http://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
-        </is>
-      </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>Protezione della popolazione</t>
-        </is>
-      </c>
+          <t>https://www.areu.lombardia.it/web/home/soreu</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr"/>
       <c r="N64" t="inlineStr"/>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>Il servizio della protezione della popolazione si occupa prevalentemente dei preparativi per i casi di emergenza e di catastrofe.
-Assicura la collaborazione con i servizi delle Amministrazioni: federale, cantonale e comunali direttamente collegate con i temi trattati dal servizio e si occupa della coordinazione fra i partner del concetto “protezione della popolazione” (polizia cantonale, Federazione cantonale ticinese dei Corpi Pompieri, Federazione cantonale ticinese dei Servizi autoambulanze, organizzazioni regionali di protezione civile, servizi tecnici cantonali, servizi dello Stato Maggiore cantonale di catastrofe, ecc…).
-Per il tramite di esercitazioni teoriche e pratiche, approfondisce con le istanze militari, la collaborazione civile-militare.</t>
-        </is>
-      </c>
-      <c r="P64" t="inlineStr">
-        <is>
-          <t>Competenza della Protezione Civile</t>
-        </is>
-      </c>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
       <c r="Q64" t="inlineStr"/>
-      <c r="R64" t="inlineStr">
-        <is>
-          <t>Presentazione</t>
-        </is>
-      </c>
+      <c r="R64" t="inlineStr"/>
       <c r="S64" t="inlineStr"/>
-      <c r="T64" t="inlineStr">
-        <is>
-          <t>Servizio della protezione della popolazione</t>
-        </is>
-      </c>
-      <c r="U64" t="inlineStr">
-        <is>
-          <t>Repubblica e Cantone Ticino</t>
-        </is>
-      </c>
-      <c r="V64" t="inlineStr">
-        <is>
-          <t>Repubblica e Cantone Ticino</t>
-        </is>
-      </c>
-      <c r="W64" t="inlineStr">
-        <is>
-          <t>https://www4.ti.ch/di/smpp/chi-siamo/servizio-della-protezione-della-popolazione/</t>
-        </is>
-      </c>
-      <c r="X64" t="inlineStr">
-        <is>
-          <t>Il significato italiano di protezione civile coincide a livello di strutture con io significato svizzero di protezione della popolazione.
-Definizioni riorganizzate da Tommaso Sansone, Politecnico di Milano.</t>
-        </is>
-      </c>
+      <c r="T64" t="inlineStr"/>
+      <c r="U64" t="inlineStr"/>
+      <c r="V64" t="inlineStr"/>
+      <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr"/>
       <c r="Y64" s="2" t="n">
-        <v>43815</v>
+        <v>43844</v>
       </c>
       <c r="Z64" t="inlineStr">
         <is>
-          <t>ITCH00025</t>
+          <t>ITCH00033</t>
         </is>
       </c>
     </row>
@@ -4753,13 +4809,13 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>SOREU dei laghi</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Il Dipartimento della protezione civile è una struttura della Presidenza del Consiglio dei Ministri. Il Dipartimento, operando in stretto raccordo con le Regioni e le Province autonome, si occupa di tutte le attività volte alla previsione e alla prevenzione dei rischi, al soccorso e all’assistenza delle popolazioni colpite da calamità, al contrasto e al superamento dell’emergenza.</t>
+          <t>La SOREU dei Laghi è il riferimento per i territori di Como, Varese, Lecco e l'area del Legnanese.</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -4768,18 +4824,18 @@
       <c r="H65" t="inlineStr"/>
       <c r="I65" t="inlineStr">
         <is>
-          <t>Dipartimento</t>
+          <t>SOREU dei Laghi</t>
         </is>
       </c>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Areu Lombardia</t>
         </is>
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>http://www.protezionecivile.gov.it/dipartimento</t>
+          <t>https://www.areu.lombardia.it/web/home/soreu-dei-laghi</t>
         </is>
       </c>
       <c r="M65" t="inlineStr"/>
@@ -4795,11 +4851,11 @@
       <c r="W65" t="inlineStr"/>
       <c r="X65" t="inlineStr"/>
       <c r="Y65" s="2" t="n">
-        <v>43817</v>
+        <v>43844</v>
       </c>
       <c r="Z65" t="inlineStr">
         <is>
-          <t>ITCH00026</t>
+          <t>ITCH00034</t>
         </is>
       </c>
     </row>
@@ -4807,52 +4863,40 @@
       <c r="A66" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B66" t="inlineStr"/>
-      <c r="C66" t="inlineStr"/>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Vigili del fuoco</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>VVF</t>
+        </is>
+      </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>La legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002 può essere considerata come la più importante legge dello stato svizzero in materia di protezione della protezione della popolazione, che costituisce quadro normativo di riferimento per altre leggi federali e cantonali in materia di protezione della popolazione. Essa disciplina principalmente due ambiti: - la collaborazione tra Confederazione e Cantoni nella protezione della popolazione. - il ruolo e i doveri degli organi e dei corpi della protezione della popolazione.</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>Normativa</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>Tommaso Sansone</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>Normativa nazionale: Legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002</t>
-        </is>
-      </c>
+          <t>Struttura operativa della protezione civile.</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
-        </is>
-      </c>
+      <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Tommaso Sansone</t>
+          <t>Alberto Bruno, Funzionario della protezione civile di regione lombardia</t>
         </is>
       </c>
       <c r="K66" t="inlineStr"/>
       <c r="L66" t="inlineStr"/>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile</t>
-        </is>
-      </c>
-      <c r="N66" t="inlineStr">
-        <is>
-          <t>LPPC</t>
-        </is>
-      </c>
-      <c r="O66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>Componente della protezione civile, costituiscono corpo civico</t>
+        </is>
+      </c>
       <c r="P66" t="inlineStr"/>
       <c r="Q66" t="inlineStr"/>
       <c r="R66" t="inlineStr"/>
@@ -4861,17 +4905,13 @@
       <c r="U66" t="inlineStr"/>
       <c r="V66" t="inlineStr"/>
       <c r="W66" t="inlineStr"/>
-      <c r="X66" t="inlineStr">
-        <is>
-          <t>definizione lato italiano, oggetto lato svizzero</t>
-        </is>
-      </c>
+      <c r="X66" t="inlineStr"/>
       <c r="Y66" s="2" t="n">
-        <v>43780</v>
+        <v>43804</v>
       </c>
       <c r="Z66" t="inlineStr">
         <is>
-          <t>ITCH00027</t>
+          <t>ITCH00035</t>
         </is>
       </c>
     </row>
@@ -4881,90 +4921,45 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Volontario di protezione civile</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr"/>
+          <t>Nucleo Unitario di Valutazione e Risposta Emergenze transfrontaliere</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>NUVRE</t>
+        </is>
+      </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Il decreto legislativo n. 1 del 2018, Codice della Protezioone Civile, include il volontariato organizzato di protezione civile iscritto nell'elenco nazionale del volontariato di protezione civile tra le strutture operative del Servizio nazionale. Il volontariato si integra con gli altri livelli territoriali di intervento previsti nell'organizzazione del sistema nazionale della protezione civile, in base al principio della sussidiarietà verticale. È inoltre attore del sistema e del proprio territorio: protegge la comunità in collaborazione con le istituzioni, in base al principio della sussidiarietà orizzontale.</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>Competenza della Protezione Civile</t>
-        </is>
-      </c>
+          <t>team transfrontaliero di coordinamento costituito congiuntamente da personale qualificato, formato e attrezzato, della protezione civile lombarda e ticinese. Esso ha il compito, durante le emergenze nei territori di confine, di operare insieme sia per la valutazione dell’evento in corso e per i reciproci possibili riflessi sui rispettivi territori, sia quali “ufficiali di collegamento” per collegare le rispettive sale operative di ambo i lati del confine, consentendo una efficiente ed efficace relazione operativa. Il NUVRE viene introdotto dal progetto Gestisco 2018-2021.</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>Home &gt; Servizio Nazionale &gt; Strutture operative &gt; Volontariato</t>
-        </is>
-      </c>
+      <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr"/>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>Dipartimento della protezione civile</t>
-        </is>
-      </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>http://www.protezionecivile.gov.it/servizio-nazionale/strutture-operative/volontariato</t>
-        </is>
-      </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>Volontario di protezione civile</t>
-        </is>
-      </c>
+      <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
       <c r="N67" t="inlineStr"/>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>La legge LPPC 2002 stabilisce che possono prestare volontariamente servizio di protezione civile: a. gli uomini prosciolti dall’obbligo di prestare servizio nella protezione civile; b. gli uomini soggetti all’obbligo militare prosciolti dall’obbligo di prestare servizio militare o civile; c. gli uomini prosciolti dall’obbligo di prestare servizio militare o civile; d. le cittadine svizzere, a partire dall’anno in cui compiono i 20 anni; e. gli stranieri domiciliati in Svizzera, a partire dall’anno in cui compiono i 20 anni. Bisogna porre attenzione al fatto che secondo la stessa legge, l’unica differenza tra un milite e un volontario (entrambi di protezione civile) è il fatto che i volontari sono prosciolti dall’obbligo di prestare servizio su domanda. Infatti, per il resto, militi e volontari hanno gli stessi diritti e doveri. 
-I diritti dei militi sono essenzialmente quattro: soldo e vitto, alloggio, trasporto gratuiti, cui si aggiungono alcune agevolazioni fiscali e indennità.</t>
-        </is>
-      </c>
-      <c r="P67" t="inlineStr">
-        <is>
-          <t>Competenza della Protezione Civile</t>
-        </is>
-      </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>Tommaso sansone</t>
-        </is>
-      </c>
-      <c r="R67" t="inlineStr">
-        <is>
-          <t>Normativa nazionale: Legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002</t>
-        </is>
-      </c>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
+      <c r="Q67" t="inlineStr"/>
+      <c r="R67" t="inlineStr"/>
       <c r="S67" t="inlineStr"/>
-      <c r="T67" t="inlineStr">
-        <is>
-          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
-        </is>
-      </c>
-      <c r="U67" t="inlineStr">
-        <is>
-          <t>Tommaso sansone</t>
-        </is>
-      </c>
+      <c r="T67" t="inlineStr"/>
+      <c r="U67" t="inlineStr"/>
       <c r="V67" t="inlineStr"/>
-      <c r="W67" t="inlineStr">
-        <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
-        </is>
-      </c>
+      <c r="W67" t="inlineStr"/>
       <c r="X67" t="inlineStr"/>
       <c r="Y67" s="2" t="n">
-        <v>43767</v>
+        <v>43774</v>
       </c>
       <c r="Z67" t="inlineStr">
         <is>
-          <t>ITCH00028</t>
+          <t>ITCH00036</t>
         </is>
       </c>
     </row>
@@ -4972,256 +4967,57 @@
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B68" t="inlineStr"/>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Centro operativo regionale</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>COR</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>E’ una struttura costituita a livello regionale nell’ambito del sistema integrato di lotta agli incendi boschivi; provvede al coordinamento di tutte le attività in materia.</t>
+        </is>
+      </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
-      <c r="I68" t="inlineStr"/>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Piano Comunale Di Emergenza - Glossario</t>
+        </is>
+      </c>
       <c r="J68" t="inlineStr"/>
-      <c r="K68" t="inlineStr"/>
-      <c r="L68" t="inlineStr"/>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>Consiglio di stato</t>
-        </is>
-      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Comune di Modena</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>https://www.comune.modena.it/ambiente/protezione-civile/piano-comunale-di-protezione-civile/scheda-19-glossario</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr"/>
       <c r="N68" t="inlineStr"/>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>Il Consiglio di Stato è l’autorità competente per: a) assicurare la condotta, l’intervento e il coordinamento delle organizzazioni partner; b) assicurare l’istruzione e la formazione, anche degli organi di condotta locali; c) promuovere l’aiuto intercomunale, così come la cooperazione intercantonale e
-transfrontaliera; d) esercitare le altre funzioni attribuitegli dalla presente legge.</t>
-        </is>
-      </c>
+      <c r="O68" t="inlineStr"/>
       <c r="P68" t="inlineStr"/>
       <c r="Q68" t="inlineStr"/>
-      <c r="R68" t="inlineStr">
-        <is>
-          <t>Art. 7</t>
-        </is>
-      </c>
+      <c r="R68" t="inlineStr"/>
       <c r="S68" t="inlineStr"/>
-      <c r="T68" t="inlineStr">
-        <is>
-          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
-        </is>
-      </c>
-      <c r="U68" t="inlineStr">
-        <is>
-          <t>Ufficio Federale della Protezione della Popolazione</t>
-        </is>
-      </c>
-      <c r="V68" t="inlineStr">
-        <is>
-          <t>Repubblica e Cantone Ticino</t>
-        </is>
-      </c>
-      <c r="W68" t="inlineStr">
-        <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/pdfatto/atto/48</t>
-        </is>
-      </c>
+      <c r="T68" t="inlineStr"/>
+      <c r="U68" t="inlineStr"/>
+      <c r="V68" t="inlineStr"/>
+      <c r="W68" t="inlineStr"/>
       <c r="X68" t="inlineStr"/>
       <c r="Y68" s="2" t="n">
-        <v>43817</v>
+        <v>43838</v>
       </c>
       <c r="Z68" t="inlineStr">
-        <is>
-          <t>ITCH00029</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B69" t="inlineStr"/>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr"/>
-      <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr"/>
-      <c r="J69" t="inlineStr"/>
-      <c r="K69" t="inlineStr"/>
-      <c r="L69" t="inlineStr"/>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>Milite</t>
-        </is>
-      </c>
-      <c r="N69" t="inlineStr"/>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>I militi svizzeri sono reclutati dall’esercito e dalla protezione civile e di norma vengono assegnati al loro cantone di domicilio, oppure ad altri cantoni, se deciso dal cantone di domicilio, cui comunque spetta la scelta. I militi, oltre ad essere arruolati in maniera ordinaria, possono essere incorporati nel personale di riserva. Se un milite entra a far parte del personale di riserva non deve essere necessariamente formato e non ha diritto a prestare servizio di protezione civile.
-Una volta reclutati e addestrasti, i militi possono essere chiamati a prestare servizio dal consiglio federale o dal cantone cui sono assegnati. Il Consiglio federale e il cantone di assegnamento possono chiamare in servizio i militi di protezione civile in caso di catastrofi e situazioni d’emergenza che colpiscono uno o più Cantoni, oppure le zone limitrofe di Paesi confinanti, oppure in caso di conflitto armato. I militi possono inoltre essere mobilitati anche in assenza di emergenza per svolgere dei lavori di ripristino di pubblica utilità. In quest’ultimo caso però, esistono dei limiti al potere di convocazione esercitato dalle autorità sui militi .</t>
-        </is>
-      </c>
-      <c r="P69" t="inlineStr"/>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>Tommaso Sansone</t>
-        </is>
-      </c>
-      <c r="R69" t="inlineStr">
-        <is>
-          <t>Normativa nazionale: Legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002</t>
-        </is>
-      </c>
-      <c r="S69" t="inlineStr"/>
-      <c r="T69" t="inlineStr">
-        <is>
-          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
-        </is>
-      </c>
-      <c r="U69" t="inlineStr">
-        <is>
-          <t>Tommaso Sansone</t>
-        </is>
-      </c>
-      <c r="V69" t="inlineStr"/>
-      <c r="W69" t="inlineStr"/>
-      <c r="X69" t="inlineStr">
-        <is>
-          <t>Definizione italiana, oggetto svizzero</t>
-        </is>
-      </c>
-      <c r="Y69" s="2" t="n">
-        <v>43766</v>
-      </c>
-      <c r="Z69" t="inlineStr">
-        <is>
-          <t>ITCH00030</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" t="inlineStr"/>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
-      <c r="I70" t="inlineStr"/>
-      <c r="J70" t="inlineStr"/>
-      <c r="K70" t="inlineStr"/>
-      <c r="L70" t="inlineStr"/>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>Legge sulla protezione della popolazione del 26 febbraio 2007</t>
-        </is>
-      </c>
-      <c r="N70" t="inlineStr">
-        <is>
-          <t>LProtPop</t>
-        </is>
-      </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>La legge cantonale del 26 febbraio 2007 è legge di maggior riferimento del Canton Ticino in materia di protezione della popolazione.
-Essa riprende alcuni argomenti già sanciti dalla legge federale LPPC del 2002, approfondisce la struttura e i compiti di alcuni organi di protezione della popolazione cantonali, quali gli organi di condotta, e descrive il concetto di stato di necessità a livello cantonale.</t>
-        </is>
-      </c>
-      <c r="P70" t="inlineStr"/>
-      <c r="Q70" t="inlineStr">
-        <is>
-          <t>Tommaso sansone</t>
-        </is>
-      </c>
-      <c r="R70" t="inlineStr">
-        <is>
-          <t>Normativa cantonale: Legge sulla protezione della popolazione (LProtPop) del 26 febbraio 2007</t>
-        </is>
-      </c>
-      <c r="S70" t="inlineStr"/>
-      <c r="T70" t="inlineStr">
-        <is>
-          <t>-- -- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
-        </is>
-      </c>
-      <c r="U70" t="inlineStr">
-        <is>
-          <t>Tommaso Sansone</t>
-        </is>
-      </c>
-      <c r="V70" t="inlineStr"/>
-      <c r="W70" t="inlineStr"/>
-      <c r="X70" t="inlineStr">
-        <is>
-          <t>definizione italiana, oggetto svizzero</t>
-        </is>
-      </c>
-      <c r="Y70" s="2" t="n">
-        <v>43817</v>
-      </c>
-      <c r="Z70" t="inlineStr">
-        <is>
-          <t>ITCH00031</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Centro operativo regionale</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>COR</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>E’ una struttura costituita a livello regionale nell’ambito del sistema integrato di lotta agli incendi boschivi; provvede al coordinamento di tutte le attività in materia.</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr"/>
-      <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>Piano Comunale Di Emergenza - Glossario</t>
-        </is>
-      </c>
-      <c r="J71" t="inlineStr"/>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>Comune di Modena</t>
-        </is>
-      </c>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>https://www.comune.modena.it/ambiente/protezione-civile/piano-comunale-di-protezione-civile/scheda-19-glossario</t>
-        </is>
-      </c>
-      <c r="M71" t="inlineStr"/>
-      <c r="N71" t="inlineStr"/>
-      <c r="O71" t="inlineStr"/>
-      <c r="P71" t="inlineStr"/>
-      <c r="Q71" t="inlineStr"/>
-      <c r="R71" t="inlineStr"/>
-      <c r="S71" t="inlineStr"/>
-      <c r="T71" t="inlineStr"/>
-      <c r="U71" t="inlineStr"/>
-      <c r="V71" t="inlineStr"/>
-      <c r="W71" t="inlineStr"/>
-      <c r="X71" t="inlineStr"/>
-      <c r="Y71" s="2" t="n">
-        <v>43838</v>
-      </c>
-      <c r="Z71" t="inlineStr">
         <is>
           <t>ITCH00040</t>
         </is>

</xml_diff>

<commit_message>
corretta grammatica in pannello di comando
</commit_message>
<xml_diff>
--- a/static/saved_dataframes/Terminologia_metaglossario.xlsx
+++ b/static/saved_dataframes/Terminologia_metaglossario.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z63"/>
+  <dimension ref="A1:Z113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -604,7 +604,7 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -668,7 +668,7 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -736,7 +736,7 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -804,7 +804,7 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -872,7 +872,7 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -1012,7 +1012,7 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1080,7 +1080,7 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1148,7 +1148,7 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -2341,7 +2341,7 @@
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Repubblica E Cantone Ticino</t>
         </is>
       </c>
       <c r="W27" t="inlineStr">
@@ -2597,12 +2597,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>IRPI</t>
+          <t>Irpi</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>IRPI CNR</t>
+          <t>Irpi Cnr</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2804,7 +2804,7 @@
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>confederazione elvetica</t>
+          <t>Confederazione Elvetica</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -2820,12 +2820,12 @@
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>Confederazion elvetica</t>
+          <t>Confederazion Elvetica</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>Confederazione elvetica</t>
+          <t>Confederazione Elvetica</t>
         </is>
       </c>
       <c r="W33" t="inlineStr">
@@ -2986,7 +2986,7 @@
       <c r="U35" t="inlineStr"/>
       <c r="V35" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Repubblica E Cantone Ticino</t>
         </is>
       </c>
       <c r="W35" t="inlineStr">
@@ -3229,7 +3229,7 @@
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>Ufficio Federale della Protezione della Popolazione</t>
+          <t>Ufficio Federale Della Protezione Della Popolazione</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
@@ -3293,7 +3293,7 @@
       </c>
       <c r="U40" t="inlineStr">
         <is>
-          <t>Ufficio Federale della Protezione della Popolazione</t>
+          <t>Ufficio Federale Della Protezione Della Popolazione</t>
         </is>
       </c>
       <c r="V40" t="inlineStr">
@@ -3366,7 +3366,7 @@
       <c r="U41" t="inlineStr"/>
       <c r="V41" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Repubblica E Cantone Ticino</t>
         </is>
       </c>
       <c r="W41" t="inlineStr">
@@ -3428,7 +3428,7 @@
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>Ufficio Federale della Protezione della Popolazione</t>
+          <t>Ufficio Federale Della Protezione Della Popolazione</t>
         </is>
       </c>
       <c r="V42" t="inlineStr">
@@ -3501,7 +3501,7 @@
       <c r="U43" t="inlineStr"/>
       <c r="V43" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Repubblica E Cantone Ticino</t>
         </is>
       </c>
       <c r="W43" t="inlineStr">
@@ -3669,7 +3669,7 @@
       <c r="U46" t="inlineStr"/>
       <c r="V46" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Repubblica E Cantone Ticino</t>
         </is>
       </c>
       <c r="W46" t="inlineStr">
@@ -3733,7 +3733,7 @@
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Repubblica E Cantone Ticino</t>
         </is>
       </c>
       <c r="W47" t="inlineStr">
@@ -3838,12 +3838,12 @@
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Repubblica E Cantone Ticino</t>
         </is>
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Repubblica E Cantone Ticino</t>
         </is>
       </c>
       <c r="W48" t="inlineStr">
@@ -3893,7 +3893,7 @@
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4013,7 +4013,7 @@
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4105,12 +4105,12 @@
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>Ufficio Federale della Protezione della Popolazione</t>
+          <t>Ufficio Federale Della Protezione Della Popolazione</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Repubblica E Cantone Ticino</t>
         </is>
       </c>
       <c r="W52" t="inlineStr">
@@ -4199,7 +4199,7 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>LProtPop</t>
+          <t>LPROTPOP</t>
         </is>
       </c>
       <c r="O54" t="inlineStr">
@@ -4281,7 +4281,7 @@
       <c r="U55" t="inlineStr"/>
       <c r="V55" t="inlineStr">
         <is>
-          <t>Repubblica e Canton Ticino</t>
+          <t>Repubblica E Canton Ticino</t>
         </is>
       </c>
       <c r="W55" t="inlineStr">
@@ -4441,7 +4441,7 @@
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Alberto Bruno, Funzionario della protezione civile di regione lombardia</t>
+          <t>Alberto Bruno, Funzionario Della Protezione Civile Di Regione Lombardia</t>
         </is>
       </c>
       <c r="K58" t="inlineStr"/>
@@ -4551,7 +4551,7 @@
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L60" t="inlineStr">
@@ -4619,7 +4619,7 @@
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
@@ -4687,7 +4687,7 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>Comune di Mozzanica</t>
+          <t>Comune Di Mozzanica</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
@@ -4756,7 +4756,7 @@
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Dipartimento Della Protezione Civile</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
@@ -4785,6 +4785,3575 @@
         </is>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Terremoto</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Intenso scuotimento della terra in un sito, come effetto del rapido spostamento di grandi porzioni di crosta terrestre in corrispondenza di una faglia posta all'interno della crosta stessa, la sorgente sismica. L'entità del terremoto dipende dalle caratteristiche geometriche della faglia, dalle modalità di propagazione della perturbazione tra la sorgente e il sito, e dalle caratteristiche lito-stratigrafiche e morfologiche di quest'ultimo.</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Geofisica</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Lettera T</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>http://www.protezionecivile.gov.it/strumenti/footer/glossario?p_p_id=DpcGlossario_WAR_DpcGlossario100SNAPSHOT&amp;p_p_lifecycle=0&amp;p_p_state=normal&amp;p_p_mode=view&amp;p_p_col_id=column-1&amp;p_p_col_count=1&amp;_DpcGlossario_WAR_DpcGlossario100SNAPSHOT_letter=T&amp;_DpcGlossario_WAR_DpcGlossario100SNAPSHOT_action=listByLetter</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Glossario – Dipartimento Della Protezione Civile</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Dipartiment Di Protezione Civile</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Dipartimento Della Protezione Civile</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>http://www.protezionecivile.gov.it/strumenti/footer/glossario</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="inlineStr"/>
+      <c r="R64" t="inlineStr"/>
+      <c r="S64" t="inlineStr"/>
+      <c r="T64" t="inlineStr"/>
+      <c r="U64" t="inlineStr"/>
+      <c r="V64" t="inlineStr"/>
+      <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>è la definizione ufficiale di terremoto proposta dal dipartimento di protezione civile</t>
+        </is>
+      </c>
+      <c r="Y64" s="2" t="n">
+        <v>43880</v>
+      </c>
+      <c r="Z64" t="inlineStr">
+        <is>
+          <t>ITCH15821271164206872</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Relazione di soccorso</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>rappresenta il documento compilato, per ogni persona soccorsa, dalle équipe di soccorso che intervengono sul territorio. La Relazione di soccorso riporta le informazioni rilevanti relative all'evento, funzionali al soccorso, (es. luogo dell'evento, tipologia di evento) nonché le informazioni relative alla persona soccorsa e al soccorso prestato (es. dati anagrafici della persona soccorsa, parametri vitali rilevati, prestazioni eventualmente effettuate).</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Ambito sanitario</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Inizio documento</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Documentazione 118</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Areu Lombardia</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>https://www.areu.lombardia.it/web/home/documentazione-118</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
+      <c r="R65" t="inlineStr"/>
+      <c r="S65" t="inlineStr"/>
+      <c r="T65" t="inlineStr"/>
+      <c r="U65" t="inlineStr"/>
+      <c r="V65" t="inlineStr"/>
+      <c r="W65" t="inlineStr"/>
+      <c r="X65" t="inlineStr">
+        <is>
+          <t>provenienza della fonte: italia, ambito sanitario. questo oggetto è stato introdotto grazie al decreto.... esiste un corrispondente in svizzera ed è la relazione detta "........</t>
+        </is>
+      </c>
+      <c r="Y65" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z65" t="inlineStr">
+        <is>
+          <t>ITCH15827985442226258</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Comitato provinciale per l’Ordine
+e la Sicurezza Pubblica</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>COSP</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Tavolo di vertice provinciale
+composto dal Prefetto, Questore,
+Comandanti Provinciali Arma dei
+Carabinieri, Guardia di Finanza,
+Vigili del Fuoco e dal Sindaco del
+Comune capoluogo</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Prefetto &gt;
+Ministero dell’Interno</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Pag. 10</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr"/>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
+      <c r="Q66" t="inlineStr"/>
+      <c r="R66" t="inlineStr"/>
+      <c r="S66" t="inlineStr"/>
+      <c r="T66" t="inlineStr"/>
+      <c r="U66" t="inlineStr"/>
+      <c r="V66" t="inlineStr"/>
+      <c r="W66" t="inlineStr"/>
+      <c r="X66" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y66" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z66" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556359</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Centro di coordinamento e
+monitoraggio dell’Evento</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>CCME</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Struttura di coordinamento
+provinciale di Safety per eventi vari</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Prefettura &gt; Ministero
+dell’Interno</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Pag. 10</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
+      <c r="Q67" t="inlineStr"/>
+      <c r="R67" t="inlineStr"/>
+      <c r="S67" t="inlineStr"/>
+      <c r="T67" t="inlineStr"/>
+      <c r="U67" t="inlineStr"/>
+      <c r="V67" t="inlineStr"/>
+      <c r="W67" t="inlineStr"/>
+      <c r="X67" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y67" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z67" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556360</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Centro Operativo Comunale</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>COC</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Struttura di coordinamento di livello
+comunale di Protezione Civile</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Comuni &gt; Prefetto</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Pag. 10</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
+      <c r="Q68" t="inlineStr"/>
+      <c r="R68" t="inlineStr"/>
+      <c r="S68" t="inlineStr"/>
+      <c r="T68" t="inlineStr"/>
+      <c r="U68" t="inlineStr"/>
+      <c r="V68" t="inlineStr"/>
+      <c r="W68" t="inlineStr"/>
+      <c r="X68" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y68" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z68" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556361</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Posto di Comando Avanzato</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>PCA</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Luogo di coordinamento sul campo
+delle forze operative in ambito di
+Soccorso pubblico e Protezione
+Civile</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Vigili del Fuoco + AREU &gt;</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Pag. 10</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
+      <c r="Q69" t="inlineStr"/>
+      <c r="R69" t="inlineStr"/>
+      <c r="S69" t="inlineStr"/>
+      <c r="T69" t="inlineStr"/>
+      <c r="U69" t="inlineStr"/>
+      <c r="V69" t="inlineStr"/>
+      <c r="W69" t="inlineStr"/>
+      <c r="X69" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y69" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z69" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556362</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Direttore Tecnico dei Soccorsi</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>DTS</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Funzionario dei VVF, dirige gli
+interventi di soccorso pubblico sul
+posto dell'emergenza, sia in campo
+di Soccorso Tecnico Urgente che di
+Protezione Civile anche avvalendosi
+del PCA</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Vigili del Fuoco</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Pag. 10</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr"/>
+      <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
+      <c r="N70" t="inlineStr"/>
+      <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
+      <c r="Q70" t="inlineStr"/>
+      <c r="R70" t="inlineStr"/>
+      <c r="S70" t="inlineStr"/>
+      <c r="T70" t="inlineStr"/>
+      <c r="U70" t="inlineStr"/>
+      <c r="V70" t="inlineStr"/>
+      <c r="W70" t="inlineStr"/>
+      <c r="X70" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y70" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z70" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556363</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Direttore dei Soccorsi Sanitari</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>DSS</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Medico di AREU, dirige i soccorsi
+sanitari sul posto dell'emergenza, sia
+in campo di Soccorso Tecnico</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>&gt; DTS VVF &gt; AREU</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Pag. 10</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr"/>
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="inlineStr"/>
+      <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
+      <c r="Q71" t="inlineStr"/>
+      <c r="R71" t="inlineStr"/>
+      <c r="S71" t="inlineStr"/>
+      <c r="T71" t="inlineStr"/>
+      <c r="U71" t="inlineStr"/>
+      <c r="V71" t="inlineStr"/>
+      <c r="W71" t="inlineStr"/>
+      <c r="X71" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y71" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z71" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556364</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Funzionario dell’Ordine Pubblico</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>FOP</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Ufficiale di Polizia Giudiziaria e di
+Pubblica Sicurezza (anche
+appartenente ai Carabinieri), dirige
+le funzioni di ordine pubblico in
+piazza. Negli interventi specifici di
+Soccorso Pubblico e Protezione
+Civile, si coordina con il DTS dei
+VVF e il DDS di AREU anche
+presso il PCA</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>&gt; Questura anche se
+Carabinieri, per la specifica
+funzione di Ordine
+Pubblico</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr"/>
+      <c r="R72" t="inlineStr"/>
+      <c r="S72" t="inlineStr"/>
+      <c r="T72" t="inlineStr"/>
+      <c r="U72" t="inlineStr"/>
+      <c r="V72" t="inlineStr"/>
+      <c r="W72" t="inlineStr"/>
+      <c r="X72" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y72" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z72" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556365</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Autorità
+territoriale di
+Protezione civile (Presidente della Regione / Sindaco
+della Città Metropolitana /
+Sindaco di Comune)</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Nell'ambito di protezione civile,
+Autorità locali elettive con potestà e
+doveri di pianificazione,
+prevenzione in ambito gestione
+dell'emergenza e suo superamento
+dell'emergenza nei propri ambiti
+giurisdizionali</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>&gt; Ente di livello superiore</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr"/>
+      <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
+      <c r="Q73" t="inlineStr"/>
+      <c r="R73" t="inlineStr"/>
+      <c r="S73" t="inlineStr"/>
+      <c r="T73" t="inlineStr"/>
+      <c r="U73" t="inlineStr"/>
+      <c r="V73" t="inlineStr"/>
+      <c r="W73" t="inlineStr"/>
+      <c r="X73" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y73" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z73" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556366</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Autorità tecnica
+provinciale di
+gestione di
+Protezione civile
+(Prefetto)</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Nell'ambito di protezione civile
+Autorità provinciale, di
+rappresentanza del Governo, con
+competenza di coordinamento e
+direzione delle operazioni nel corso
+delle emergenze</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>&gt; Dipartimento della
+Protezione civile
+Si coordina con il
+Presidente della Regione</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="inlineStr"/>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
+      <c r="Q74" t="inlineStr"/>
+      <c r="R74" t="inlineStr"/>
+      <c r="S74" t="inlineStr"/>
+      <c r="T74" t="inlineStr"/>
+      <c r="U74" t="inlineStr"/>
+      <c r="V74" t="inlineStr"/>
+      <c r="W74" t="inlineStr"/>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y74" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z74" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556367</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Funzionario di Protezione Civile</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Pubblici funzionari appartenenti ai
+Servizi di Protezione Civile di
+Regione, Prefettura, Città
+Metropolitana /Province e Comuni</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>&gt; Enti Pubblici di rispettiva
+dipendenza</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr"/>
+      <c r="L75" t="inlineStr"/>
+      <c r="M75" t="inlineStr"/>
+      <c r="N75" t="inlineStr"/>
+      <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
+      <c r="Q75" t="inlineStr"/>
+      <c r="R75" t="inlineStr"/>
+      <c r="S75" t="inlineStr"/>
+      <c r="T75" t="inlineStr"/>
+      <c r="U75" t="inlineStr"/>
+      <c r="V75" t="inlineStr"/>
+      <c r="W75" t="inlineStr"/>
+      <c r="X75" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y75" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z75" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556368</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Coordinatore Tecnico dei
+Volontari</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>CTV</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Volontari esperti di Protezione
+Civile, deputati al coordinamento
+operativo del volontariato di
+Protezione Civile, secondo le
+direttive dei Funzionari di
+Protezione Civile</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>&gt; Funzionari di Protezione
+Civile</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr"/>
+      <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
+      <c r="N76" t="inlineStr"/>
+      <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
+      <c r="Q76" t="inlineStr"/>
+      <c r="R76" t="inlineStr"/>
+      <c r="S76" t="inlineStr"/>
+      <c r="T76" t="inlineStr"/>
+      <c r="U76" t="inlineStr"/>
+      <c r="V76" t="inlineStr"/>
+      <c r="W76" t="inlineStr"/>
+      <c r="X76" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y76" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z76" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556369</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Dipartimento nazionale di Protezione Civile</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>DPC</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Presidenza Consiglio dei
+Ministri</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr"/>
+      <c r="L77" t="inlineStr"/>
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="inlineStr"/>
+      <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
+      <c r="Q77" t="inlineStr"/>
+      <c r="R77" t="inlineStr"/>
+      <c r="S77" t="inlineStr"/>
+      <c r="T77" t="inlineStr"/>
+      <c r="U77" t="inlineStr"/>
+      <c r="V77" t="inlineStr"/>
+      <c r="W77" t="inlineStr"/>
+      <c r="X77" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y77" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z77" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556370</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Prefetture -Uffici Territoriali del
+Governo</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>UTG</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Ministero dell’Interno
+&gt; DPC per la specificità di
+PC</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr"/>
+      <c r="L78" t="inlineStr"/>
+      <c r="M78" t="inlineStr"/>
+      <c r="N78" t="inlineStr"/>
+      <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
+      <c r="Q78" t="inlineStr"/>
+      <c r="R78" t="inlineStr"/>
+      <c r="S78" t="inlineStr"/>
+      <c r="T78" t="inlineStr"/>
+      <c r="U78" t="inlineStr"/>
+      <c r="V78" t="inlineStr"/>
+      <c r="W78" t="inlineStr"/>
+      <c r="X78" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y78" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z78" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556371</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Corpo Nazionale dei Vigili del
+Fuoco</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>CN VVF O VVF</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Dip. Vigili del Fuoco, della
+Difesa Civile e del Soccorso
+del Ministero dell’Interno</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr"/>
+      <c r="L79" t="inlineStr"/>
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="inlineStr"/>
+      <c r="O79" t="inlineStr"/>
+      <c r="P79" t="inlineStr"/>
+      <c r="Q79" t="inlineStr"/>
+      <c r="R79" t="inlineStr"/>
+      <c r="S79" t="inlineStr"/>
+      <c r="T79" t="inlineStr"/>
+      <c r="U79" t="inlineStr"/>
+      <c r="V79" t="inlineStr"/>
+      <c r="W79" t="inlineStr"/>
+      <c r="X79" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y79" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z79" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556372</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Sistema di Protezione Civile</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>SPC O PC</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="inlineStr"/>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr"/>
+      <c r="L80" t="inlineStr"/>
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="inlineStr"/>
+      <c r="O80" t="inlineStr"/>
+      <c r="P80" t="inlineStr"/>
+      <c r="Q80" t="inlineStr"/>
+      <c r="R80" t="inlineStr"/>
+      <c r="S80" t="inlineStr"/>
+      <c r="T80" t="inlineStr"/>
+      <c r="U80" t="inlineStr"/>
+      <c r="V80" t="inlineStr"/>
+      <c r="W80" t="inlineStr"/>
+      <c r="X80" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y80" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z80" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556373</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Forze di Polizia</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>FF.PP.</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Forze di polizia statuali</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr"/>
+      <c r="L81" t="inlineStr"/>
+      <c r="M81" t="inlineStr"/>
+      <c r="N81" t="inlineStr"/>
+      <c r="O81" t="inlineStr"/>
+      <c r="P81" t="inlineStr"/>
+      <c r="Q81" t="inlineStr"/>
+      <c r="R81" t="inlineStr"/>
+      <c r="S81" t="inlineStr"/>
+      <c r="T81" t="inlineStr"/>
+      <c r="U81" t="inlineStr"/>
+      <c r="V81" t="inlineStr"/>
+      <c r="W81" t="inlineStr"/>
+      <c r="X81" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y81" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z81" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556374</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Polizia di Stato</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Forze di polizia statuali</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Dip Pubblica Sicurezza del
+Ministero dell’Interno</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr"/>
+      <c r="L82" t="inlineStr"/>
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="inlineStr"/>
+      <c r="O82" t="inlineStr"/>
+      <c r="P82" t="inlineStr"/>
+      <c r="Q82" t="inlineStr"/>
+      <c r="R82" t="inlineStr"/>
+      <c r="S82" t="inlineStr"/>
+      <c r="T82" t="inlineStr"/>
+      <c r="U82" t="inlineStr"/>
+      <c r="V82" t="inlineStr"/>
+      <c r="W82" t="inlineStr"/>
+      <c r="X82" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y82" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z82" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556375</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Polizia ferroviaria</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>POLFER</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Forze di polizia statuali
+Specialità di PS</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Dip Pubblica Sicurezza del
+Ministero dell’Interno</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr"/>
+      <c r="L83" t="inlineStr"/>
+      <c r="M83" t="inlineStr"/>
+      <c r="N83" t="inlineStr"/>
+      <c r="O83" t="inlineStr"/>
+      <c r="P83" t="inlineStr"/>
+      <c r="Q83" t="inlineStr"/>
+      <c r="R83" t="inlineStr"/>
+      <c r="S83" t="inlineStr"/>
+      <c r="T83" t="inlineStr"/>
+      <c r="U83" t="inlineStr"/>
+      <c r="V83" t="inlineStr"/>
+      <c r="W83" t="inlineStr"/>
+      <c r="X83" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y83" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z83" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556376</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Polizia Stradale</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>POLSTRADA</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Forze di polizia statuali
+Specialità di PS</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Dip Pubblica Sicurezza del
+Ministero dell’Interno</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr"/>
+      <c r="L84" t="inlineStr"/>
+      <c r="M84" t="inlineStr"/>
+      <c r="N84" t="inlineStr"/>
+      <c r="O84" t="inlineStr"/>
+      <c r="P84" t="inlineStr"/>
+      <c r="Q84" t="inlineStr"/>
+      <c r="R84" t="inlineStr"/>
+      <c r="S84" t="inlineStr"/>
+      <c r="T84" t="inlineStr"/>
+      <c r="U84" t="inlineStr"/>
+      <c r="V84" t="inlineStr"/>
+      <c r="W84" t="inlineStr"/>
+      <c r="X84" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y84" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z84" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556377</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Polizia di Frontiera</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>POLARIA</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Forze di polizia statuali
+Specialità di PS</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Dip Pubblica Sicurezza del
+Ministero dell’Interno</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr"/>
+      <c r="L85" t="inlineStr"/>
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="inlineStr"/>
+      <c r="O85" t="inlineStr"/>
+      <c r="P85" t="inlineStr"/>
+      <c r="Q85" t="inlineStr"/>
+      <c r="R85" t="inlineStr"/>
+      <c r="S85" t="inlineStr"/>
+      <c r="T85" t="inlineStr"/>
+      <c r="U85" t="inlineStr"/>
+      <c r="V85" t="inlineStr"/>
+      <c r="W85" t="inlineStr"/>
+      <c r="X85" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y85" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z85" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556378</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Polizia Postale e delle
+Comunicazioni</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>POLPOSTA</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Forze di polizia statuali
+Specialità di PS</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Dip Pubblica Sicurezza del
+Ministero dell’Interno</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr"/>
+      <c r="L86" t="inlineStr"/>
+      <c r="M86" t="inlineStr"/>
+      <c r="N86" t="inlineStr"/>
+      <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr"/>
+      <c r="Q86" t="inlineStr"/>
+      <c r="R86" t="inlineStr"/>
+      <c r="S86" t="inlineStr"/>
+      <c r="T86" t="inlineStr"/>
+      <c r="U86" t="inlineStr"/>
+      <c r="V86" t="inlineStr"/>
+      <c r="W86" t="inlineStr"/>
+      <c r="X86" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y86" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z86" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556379</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Arma dei Carabinieri</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Forze di polizia statuali e Forza
+Armata</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Ministero della Difesa
+&gt; Dip Pubblica Sicurezza
+per la specificità di PS</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr"/>
+      <c r="L87" t="inlineStr"/>
+      <c r="M87" t="inlineStr"/>
+      <c r="N87" t="inlineStr"/>
+      <c r="O87" t="inlineStr"/>
+      <c r="P87" t="inlineStr"/>
+      <c r="Q87" t="inlineStr"/>
+      <c r="R87" t="inlineStr"/>
+      <c r="S87" t="inlineStr"/>
+      <c r="T87" t="inlineStr"/>
+      <c r="U87" t="inlineStr"/>
+      <c r="V87" t="inlineStr"/>
+      <c r="W87" t="inlineStr"/>
+      <c r="X87" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y87" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z87" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556380</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Guardia di Finanza</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>GDF</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Forze di polizia statuali ad
+ordinamento militare</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Ministero del Tesoro
+&gt; Dip Pubblica Sicurezza
+per la specificità di PS</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr"/>
+      <c r="L88" t="inlineStr"/>
+      <c r="M88" t="inlineStr"/>
+      <c r="N88" t="inlineStr"/>
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
+      <c r="Q88" t="inlineStr"/>
+      <c r="R88" t="inlineStr"/>
+      <c r="S88" t="inlineStr"/>
+      <c r="T88" t="inlineStr"/>
+      <c r="U88" t="inlineStr"/>
+      <c r="V88" t="inlineStr"/>
+      <c r="W88" t="inlineStr"/>
+      <c r="X88" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y88" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z88" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556381</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Forze Armate</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>FF.AA.</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Complessivo del Forze della Difesa</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Ministero della Difesa</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr"/>
+      <c r="L89" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
+      <c r="R89" t="inlineStr"/>
+      <c r="S89" t="inlineStr"/>
+      <c r="T89" t="inlineStr"/>
+      <c r="U89" t="inlineStr"/>
+      <c r="V89" t="inlineStr"/>
+      <c r="W89" t="inlineStr"/>
+      <c r="X89" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y89" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z89" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556382</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Esercito Italiano</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>EI</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Forze di difesa</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Ministero della Difesa</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr"/>
+      <c r="L90" t="inlineStr"/>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr"/>
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="inlineStr"/>
+      <c r="R90" t="inlineStr"/>
+      <c r="S90" t="inlineStr"/>
+      <c r="T90" t="inlineStr"/>
+      <c r="U90" t="inlineStr"/>
+      <c r="V90" t="inlineStr"/>
+      <c r="W90" t="inlineStr"/>
+      <c r="X90" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y90" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z90" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556383</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Comando Militare Esercito</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>EI - CME</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Forze di difesa</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Ministero della Difesa</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr"/>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr"/>
+      <c r="L91" t="inlineStr"/>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr"/>
+      <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
+      <c r="Q91" t="inlineStr"/>
+      <c r="R91" t="inlineStr"/>
+      <c r="S91" t="inlineStr"/>
+      <c r="T91" t="inlineStr"/>
+      <c r="U91" t="inlineStr"/>
+      <c r="V91" t="inlineStr"/>
+      <c r="W91" t="inlineStr"/>
+      <c r="X91" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y91" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z91" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556384</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Comando Truppe Alpine Esercito</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>EI –C.DO TA</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Forze di difesa</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Ministero della Difesa</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr"/>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Pag. 11</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr"/>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr"/>
+      <c r="L92" t="inlineStr"/>
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="inlineStr"/>
+      <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
+      <c r="Q92" t="inlineStr"/>
+      <c r="R92" t="inlineStr"/>
+      <c r="S92" t="inlineStr"/>
+      <c r="T92" t="inlineStr"/>
+      <c r="U92" t="inlineStr"/>
+      <c r="V92" t="inlineStr"/>
+      <c r="W92" t="inlineStr"/>
+      <c r="X92" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y92" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z92" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556385</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Aereonautica Militare</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>AM</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Forze di difesa</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Ministero della Difesa</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr"/>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr"/>
+      <c r="L93" t="inlineStr"/>
+      <c r="M93" t="inlineStr"/>
+      <c r="N93" t="inlineStr"/>
+      <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
+      <c r="Q93" t="inlineStr"/>
+      <c r="R93" t="inlineStr"/>
+      <c r="S93" t="inlineStr"/>
+      <c r="T93" t="inlineStr"/>
+      <c r="U93" t="inlineStr"/>
+      <c r="V93" t="inlineStr"/>
+      <c r="W93" t="inlineStr"/>
+      <c r="X93" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y93" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z93" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556386</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Enti Locali</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>EE.LL.</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Comuni, Province, Città
+Metropolitane, Comunità
+Montante</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Enti Locali</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr"/>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr"/>
+      <c r="L94" t="inlineStr"/>
+      <c r="M94" t="inlineStr"/>
+      <c r="N94" t="inlineStr"/>
+      <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
+      <c r="Q94" t="inlineStr"/>
+      <c r="R94" t="inlineStr"/>
+      <c r="S94" t="inlineStr"/>
+      <c r="T94" t="inlineStr"/>
+      <c r="U94" t="inlineStr"/>
+      <c r="V94" t="inlineStr"/>
+      <c r="W94" t="inlineStr"/>
+      <c r="X94" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y94" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z94" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556387</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Regione Lombardia</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>RL</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Ente Pubblico regionale</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Enti Locali</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr"/>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr"/>
+      <c r="L95" t="inlineStr"/>
+      <c r="M95" t="inlineStr"/>
+      <c r="N95" t="inlineStr"/>
+      <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
+      <c r="Q95" t="inlineStr"/>
+      <c r="R95" t="inlineStr"/>
+      <c r="S95" t="inlineStr"/>
+      <c r="T95" t="inlineStr"/>
+      <c r="U95" t="inlineStr"/>
+      <c r="V95" t="inlineStr"/>
+      <c r="W95" t="inlineStr"/>
+      <c r="X95" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y95" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z95" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556388</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Polizie Locali o Polizia Locale</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>PPLL O PL</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Corpi di Polizia in campo ai
+Comuni e alle Province</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Enti Locali</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr"/>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr"/>
+      <c r="L96" t="inlineStr"/>
+      <c r="M96" t="inlineStr"/>
+      <c r="N96" t="inlineStr"/>
+      <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
+      <c r="Q96" t="inlineStr"/>
+      <c r="R96" t="inlineStr"/>
+      <c r="S96" t="inlineStr"/>
+      <c r="T96" t="inlineStr"/>
+      <c r="U96" t="inlineStr"/>
+      <c r="V96" t="inlineStr"/>
+      <c r="W96" t="inlineStr"/>
+      <c r="X96" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y96" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z96" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556389</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Direzione Generale / Direzione
+Centrale / Direzione Specialistica /
+Unità Organizzativa</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>DG / DC/ DS /UO</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Articolazione del sistema
+ammnistrativo in uso alle
+pubbliche amministrazioni civili</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Enti Locali</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr"/>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr"/>
+      <c r="L97" t="inlineStr"/>
+      <c r="M97" t="inlineStr"/>
+      <c r="N97" t="inlineStr"/>
+      <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr"/>
+      <c r="Q97" t="inlineStr"/>
+      <c r="R97" t="inlineStr"/>
+      <c r="S97" t="inlineStr"/>
+      <c r="T97" t="inlineStr"/>
+      <c r="U97" t="inlineStr"/>
+      <c r="V97" t="inlineStr"/>
+      <c r="W97" t="inlineStr"/>
+      <c r="X97" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y97" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z97" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556390</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Sala Operativa Regionale</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>SOR</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Struttura coordinamento
+regionale del Sistema di
+Protezione Civile</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Regione Lombardia
+D.G. Territorio e
+Protezione Civile</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr"/>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr"/>
+      <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr"/>
+      <c r="N98" t="inlineStr"/>
+      <c r="O98" t="inlineStr"/>
+      <c r="P98" t="inlineStr"/>
+      <c r="Q98" t="inlineStr"/>
+      <c r="R98" t="inlineStr"/>
+      <c r="S98" t="inlineStr"/>
+      <c r="T98" t="inlineStr"/>
+      <c r="U98" t="inlineStr"/>
+      <c r="V98" t="inlineStr"/>
+      <c r="W98" t="inlineStr"/>
+      <c r="X98" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y98" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z98" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556391</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Centro Funzionale di
+Monitoraggio dei Rischi e Sistema
+di Allertamento</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>CF</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Struttura di monitoraggio
+deputata alle diramazione
+dell'allerte
+Sistema di Protezione Civile</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Regione Lombardia
+D.G. Territorio e
+Protezione Civile</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr"/>
+      <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
+      <c r="Q99" t="inlineStr"/>
+      <c r="R99" t="inlineStr"/>
+      <c r="S99" t="inlineStr"/>
+      <c r="T99" t="inlineStr"/>
+      <c r="U99" t="inlineStr"/>
+      <c r="V99" t="inlineStr"/>
+      <c r="W99" t="inlineStr"/>
+      <c r="X99" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y99" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z99" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556392</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Colonna Mobile Regionale</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>CMR</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Struttura operativa di risorse
+regionali di Protezione civile</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Regione Lombardia</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr"/>
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr"/>
+      <c r="N100" t="inlineStr"/>
+      <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
+      <c r="Q100" t="inlineStr"/>
+      <c r="R100" t="inlineStr"/>
+      <c r="S100" t="inlineStr"/>
+      <c r="T100" t="inlineStr"/>
+      <c r="U100" t="inlineStr"/>
+      <c r="V100" t="inlineStr"/>
+      <c r="W100" t="inlineStr"/>
+      <c r="X100" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y100" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z100" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556393</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Colonna Mobile Provinciale</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>CMP</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Struttura operativa di risorse
+regionali di Protezione civile</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Regione Lombardia</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr"/>
+      <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="inlineStr"/>
+      <c r="O101" t="inlineStr"/>
+      <c r="P101" t="inlineStr"/>
+      <c r="Q101" t="inlineStr"/>
+      <c r="R101" t="inlineStr"/>
+      <c r="S101" t="inlineStr"/>
+      <c r="T101" t="inlineStr"/>
+      <c r="U101" t="inlineStr"/>
+      <c r="V101" t="inlineStr"/>
+      <c r="W101" t="inlineStr"/>
+      <c r="X101" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y101" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z101" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556394</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Azienda Socio Sanitaria
+Territoriale (Ospedali)</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>ASST</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Aziende Ospedaliere</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Regione Lombardia
+D.G. Welfare</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr"/>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr"/>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr"/>
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr"/>
+      <c r="N102" t="inlineStr"/>
+      <c r="O102" t="inlineStr"/>
+      <c r="P102" t="inlineStr"/>
+      <c r="Q102" t="inlineStr"/>
+      <c r="R102" t="inlineStr"/>
+      <c r="S102" t="inlineStr"/>
+      <c r="T102" t="inlineStr"/>
+      <c r="U102" t="inlineStr"/>
+      <c r="V102" t="inlineStr"/>
+      <c r="W102" t="inlineStr"/>
+      <c r="X102" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y102" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z102" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556395</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Agenzia Tutela Salute</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>ATS</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Servizi sanitari del territorio</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Regione Lombardia
+D.G. Welfare</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr"/>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr"/>
+      <c r="L103" t="inlineStr"/>
+      <c r="M103" t="inlineStr"/>
+      <c r="N103" t="inlineStr"/>
+      <c r="O103" t="inlineStr"/>
+      <c r="P103" t="inlineStr"/>
+      <c r="Q103" t="inlineStr"/>
+      <c r="R103" t="inlineStr"/>
+      <c r="S103" t="inlineStr"/>
+      <c r="T103" t="inlineStr"/>
+      <c r="U103" t="inlineStr"/>
+      <c r="V103" t="inlineStr"/>
+      <c r="W103" t="inlineStr"/>
+      <c r="X103" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y103" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z103" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556396</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Azienda Regionale Emergenze e
+Urgenze</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>AREU</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Soccorso sanitario</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Regione Lombardia
+D.G. Welfare</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr"/>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr"/>
+      <c r="L104" t="inlineStr"/>
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="inlineStr"/>
+      <c r="O104" t="inlineStr"/>
+      <c r="P104" t="inlineStr"/>
+      <c r="Q104" t="inlineStr"/>
+      <c r="R104" t="inlineStr"/>
+      <c r="S104" t="inlineStr"/>
+      <c r="T104" t="inlineStr"/>
+      <c r="U104" t="inlineStr"/>
+      <c r="V104" t="inlineStr"/>
+      <c r="W104" t="inlineStr"/>
+      <c r="X104" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y104" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z104" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556397</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Ufficio Regionale del Territorio</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>UTR</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Regione Lombardia
+D.G. Welfare</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr"/>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr"/>
+      <c r="L105" t="inlineStr"/>
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="inlineStr"/>
+      <c r="O105" t="inlineStr"/>
+      <c r="P105" t="inlineStr"/>
+      <c r="Q105" t="inlineStr"/>
+      <c r="R105" t="inlineStr"/>
+      <c r="S105" t="inlineStr"/>
+      <c r="T105" t="inlineStr"/>
+      <c r="U105" t="inlineStr"/>
+      <c r="V105" t="inlineStr"/>
+      <c r="W105" t="inlineStr"/>
+      <c r="X105" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y105" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z105" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556398</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Associazione Nazionale Alpini</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>ANA</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Associazione Combattentistica e
+d'Arma</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Associazione Combattentistica e
+d’Arma</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr"/>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr"/>
+      <c r="L106" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
+      <c r="P106" t="inlineStr"/>
+      <c r="Q106" t="inlineStr"/>
+      <c r="R106" t="inlineStr"/>
+      <c r="S106" t="inlineStr"/>
+      <c r="T106" t="inlineStr"/>
+      <c r="U106" t="inlineStr"/>
+      <c r="V106" t="inlineStr"/>
+      <c r="W106" t="inlineStr"/>
+      <c r="X106" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y106" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z106" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556399</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Comitato Organizzativo Adunata
+Alpini</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>COA ANA</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Struttura organizzativa dedicata</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>&gt; A.N.A</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr"/>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K107" t="inlineStr"/>
+      <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
+      <c r="P107" t="inlineStr"/>
+      <c r="Q107" t="inlineStr"/>
+      <c r="R107" t="inlineStr"/>
+      <c r="S107" t="inlineStr"/>
+      <c r="T107" t="inlineStr"/>
+      <c r="U107" t="inlineStr"/>
+      <c r="V107" t="inlineStr"/>
+      <c r="W107" t="inlineStr"/>
+      <c r="X107" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y107" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z107" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556400</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Comitato di Coordinamento
+provinciale del Volontariato di
+Protezione Civile</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>CCV</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Sistema di Protezione Civile
+Livello provinciale</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Terzo Settore
+CMM e Province della
+Regione Lombardia</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr"/>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr"/>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr"/>
+      <c r="L108" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
+      <c r="P108" t="inlineStr"/>
+      <c r="Q108" t="inlineStr"/>
+      <c r="R108" t="inlineStr"/>
+      <c r="S108" t="inlineStr"/>
+      <c r="T108" t="inlineStr"/>
+      <c r="U108" t="inlineStr"/>
+      <c r="V108" t="inlineStr"/>
+      <c r="W108" t="inlineStr"/>
+      <c r="X108" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y108" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z108" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556401</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Organizzazione di volontariato di
+Protezione Civile</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>OVPC</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Sistema di Protezione Civile
+livello, locale, regionale e
+nazionale</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Terzo Settore</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr"/>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>Pag. 12</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr"/>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr"/>
+      <c r="L109" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
+      <c r="Q109" t="inlineStr"/>
+      <c r="R109" t="inlineStr"/>
+      <c r="S109" t="inlineStr"/>
+      <c r="T109" t="inlineStr"/>
+      <c r="U109" t="inlineStr"/>
+      <c r="V109" t="inlineStr"/>
+      <c r="W109" t="inlineStr"/>
+      <c r="X109" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y109" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z109" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556402</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Comando</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>C.DO</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Organizzazione militare</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr"/>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Pag. 13</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr"/>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr"/>
+      <c r="L110" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
+      <c r="P110" t="inlineStr"/>
+      <c r="Q110" t="inlineStr"/>
+      <c r="R110" t="inlineStr"/>
+      <c r="S110" t="inlineStr"/>
+      <c r="T110" t="inlineStr"/>
+      <c r="U110" t="inlineStr"/>
+      <c r="V110" t="inlineStr"/>
+      <c r="W110" t="inlineStr"/>
+      <c r="X110" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y110" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z110" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556403</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Gruppo</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>GR.</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Organizzazione militare</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Pag. 13</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr"/>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr"/>
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
+      <c r="P111" t="inlineStr"/>
+      <c r="Q111" t="inlineStr"/>
+      <c r="R111" t="inlineStr"/>
+      <c r="S111" t="inlineStr"/>
+      <c r="T111" t="inlineStr"/>
+      <c r="U111" t="inlineStr"/>
+      <c r="V111" t="inlineStr"/>
+      <c r="W111" t="inlineStr"/>
+      <c r="X111" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y111" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z111" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556404</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Compagnia</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>COMP.</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Organizzazione militare</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr"/>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>Pag. 13</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr"/>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr"/>
+      <c r="L112" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
+      <c r="N112" t="inlineStr"/>
+      <c r="O112" t="inlineStr"/>
+      <c r="P112" t="inlineStr"/>
+      <c r="Q112" t="inlineStr"/>
+      <c r="R112" t="inlineStr"/>
+      <c r="S112" t="inlineStr"/>
+      <c r="T112" t="inlineStr"/>
+      <c r="U112" t="inlineStr"/>
+      <c r="V112" t="inlineStr"/>
+      <c r="W112" t="inlineStr"/>
+      <c r="X112" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y112" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z112" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556405</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Stazione</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>STZ.</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr"/>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Organizzazione militare</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr"/>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Pag. 13</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr"/>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>92° Adunata Nazionale Alpini - Piano del sistema di safety in ambito metropolitano</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>Prefettura Di Miliano; Comando Provinciale Vv.F Di Milano, Regione Lombardia - D.G. Territorio E Protezione Civile / D.G. Welfare / A.R.E.U. 118
+Lombardia / A.T.S. Agenzia Tutela Salute Della Citta Metropolitana Di Milano Città Metropolitana Di Milano – D.T.O. Protezione Civile; Comune Di
+Milano – D.S. Protezione Civile; Associazione Nazionale Alpini - C.O.A 92^ Milano</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr"/>
+      <c r="L113" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="inlineStr"/>
+      <c r="O113" t="inlineStr"/>
+      <c r="P113" t="inlineStr"/>
+      <c r="Q113" t="inlineStr"/>
+      <c r="R113" t="inlineStr"/>
+      <c r="S113" t="inlineStr"/>
+      <c r="T113" t="inlineStr"/>
+      <c r="U113" t="inlineStr"/>
+      <c r="V113" t="inlineStr"/>
+      <c r="W113" t="inlineStr"/>
+      <c r="X113" t="inlineStr">
+        <is>
+          <t>il documento fonte è un glossario presente all'interno del piano del "sistema di safety in ambito metropolitano". È stato consegnato da Regione Lomnbardia al Politecnico di Milano in ambito del progetto Gestisco a fine aprile 2019. Il glossario fa riferimento a elementi di protezione civile e forze dell'ordine solamente di parte italiana.</t>
+        </is>
+      </c>
+      <c r="Y113" s="2" t="n">
+        <v>43888</v>
+      </c>
+      <c r="Z113" t="inlineStr">
+        <is>
+          <t>ITCH15828235508556406</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>